<commit_message>
Regen results by ignoring CIs for health. Rel #120
</commit_message>
<xml_diff>
--- a/results/multi_city/AP/desc_stats.xlsx
+++ b/results/multi_city/AP/desc_stats.xlsx
@@ -624,7 +624,7 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>12.9</t>
+          <t>39.6</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -771,7 +771,7 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>20.9</t>
+          <t>21.6</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
@@ -918,7 +918,7 @@
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>20.5</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
@@ -1065,7 +1065,7 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>4.9</t>
+          <t>0.7</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
@@ -1212,7 +1212,7 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>8.8</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
@@ -1359,7 +1359,7 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>43.6</t>
+          <t>17.6</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
@@ -5829,19 +5829,19 @@
         </is>
       </c>
       <c r="B107">
-        <v>48.7</v>
+        <v>33.3</v>
       </c>
       <c r="C107">
-        <v>47.4</v>
+        <v>32.4</v>
       </c>
       <c r="D107">
-        <v>47.4</v>
+        <v>32.4</v>
       </c>
       <c r="E107">
-        <v>51</v>
+        <v>34.9</v>
       </c>
       <c r="F107">
-        <v>47.4</v>
+        <v>32.38</v>
       </c>
       <c r="G107">
         <v>0</v>
@@ -5862,22 +5862,22 @@
         </is>
       </c>
       <c r="B108">
-        <v>48.4</v>
+        <v>33.1</v>
       </c>
       <c r="C108">
-        <v>46.9</v>
+        <v>32</v>
       </c>
       <c r="D108">
-        <v>46.9</v>
+        <v>32</v>
       </c>
       <c r="E108">
-        <v>51.5</v>
+        <v>35.2</v>
       </c>
       <c r="F108">
-        <v>46.91</v>
+        <v>32.04</v>
       </c>
       <c r="G108">
-        <v>-0.49</v>
+        <v>-0.34</v>
       </c>
       <c r="H108">
         <v>2117283.2</v>
@@ -5895,22 +5895,22 @@
         </is>
       </c>
       <c r="B109">
-        <v>53.6</v>
+        <v>36.6</v>
       </c>
       <c r="C109">
-        <v>52.2</v>
+        <v>35.6</v>
       </c>
       <c r="D109">
-        <v>52.2</v>
+        <v>35.6</v>
       </c>
       <c r="E109">
-        <v>56.2</v>
+        <v>38.4</v>
       </c>
       <c r="F109">
-        <v>52.16</v>
+        <v>35.63</v>
       </c>
       <c r="G109">
-        <v>4.76</v>
+        <v>3.25</v>
       </c>
       <c r="H109">
         <v>2628058.3</v>
@@ -5928,22 +5928,22 @@
         </is>
       </c>
       <c r="B110">
-        <v>48.2</v>
+        <v>32.9</v>
       </c>
       <c r="C110">
-        <v>46.9</v>
+        <v>32</v>
       </c>
       <c r="D110">
-        <v>46.9</v>
+        <v>32</v>
       </c>
       <c r="E110">
-        <v>50.5</v>
+        <v>34.5</v>
       </c>
       <c r="F110">
-        <v>46.89</v>
+        <v>32.03</v>
       </c>
       <c r="G110">
-        <v>-0.51</v>
+        <v>-0.35</v>
       </c>
       <c r="H110">
         <v>2108705.5</v>
@@ -5961,22 +5961,22 @@
         </is>
       </c>
       <c r="B111">
-        <v>47.5</v>
+        <v>32.4</v>
       </c>
       <c r="C111">
-        <v>46.2</v>
+        <v>31.6</v>
       </c>
       <c r="D111">
-        <v>46.2</v>
+        <v>31.6</v>
       </c>
       <c r="E111">
-        <v>49.7</v>
+        <v>34</v>
       </c>
       <c r="F111">
-        <v>46.2</v>
+        <v>31.56</v>
       </c>
       <c r="G111">
-        <v>-1.2</v>
+        <v>-0.82</v>
       </c>
       <c r="H111">
         <v>2093151.2</v>
@@ -5994,19 +5994,19 @@
         </is>
       </c>
       <c r="B112">
-        <v>24.7</v>
+        <v>15.9</v>
       </c>
       <c r="C112">
-        <v>23.1</v>
+        <v>14.9</v>
       </c>
       <c r="D112">
-        <v>24</v>
+        <v>15.4</v>
       </c>
       <c r="E112">
-        <v>26.5</v>
+        <v>17</v>
       </c>
       <c r="F112">
-        <v>23.07</v>
+        <v>14.86</v>
       </c>
       <c r="G112">
         <v>0</v>
@@ -6027,22 +6027,22 @@
         </is>
       </c>
       <c r="B113">
-        <v>24.6</v>
+        <v>15.8</v>
       </c>
       <c r="C113">
-        <v>22.8</v>
+        <v>14.7</v>
       </c>
       <c r="D113">
-        <v>23.8</v>
+        <v>15.4</v>
       </c>
       <c r="E113">
-        <v>26.5</v>
+        <v>17.1</v>
       </c>
       <c r="F113">
-        <v>22.84</v>
+        <v>14.72</v>
       </c>
       <c r="G113">
-        <v>-0.23</v>
+        <v>-0.14</v>
       </c>
       <c r="H113">
         <v>1749135.7</v>
@@ -6060,22 +6060,22 @@
         </is>
       </c>
       <c r="B114">
-        <v>24.3</v>
+        <v>15.8</v>
       </c>
       <c r="C114">
-        <v>22.7</v>
+        <v>14.8</v>
       </c>
       <c r="D114">
-        <v>23.5</v>
+        <v>15.3</v>
       </c>
       <c r="E114">
-        <v>26.1</v>
+        <v>17</v>
       </c>
       <c r="F114">
-        <v>22.66</v>
+        <v>14.78</v>
       </c>
       <c r="G114">
-        <v>-0.41</v>
+        <v>-0.08</v>
       </c>
       <c r="H114">
         <v>1817428.1</v>
@@ -6093,22 +6093,22 @@
         </is>
       </c>
       <c r="B115">
-        <v>24.7</v>
+        <v>15.8</v>
       </c>
       <c r="C115">
-        <v>23.1</v>
+        <v>14.8</v>
       </c>
       <c r="D115">
-        <v>24</v>
+        <v>15.4</v>
       </c>
       <c r="E115">
-        <v>26.4</v>
+        <v>16.9</v>
       </c>
       <c r="F115">
-        <v>23.14</v>
+        <v>14.83</v>
       </c>
       <c r="G115">
-        <v>0.07000000000000001</v>
+        <v>-0.03</v>
       </c>
       <c r="H115">
         <v>1735620.8</v>
@@ -6126,22 +6126,22 @@
         </is>
       </c>
       <c r="B116">
-        <v>28.9</v>
+        <v>16.1</v>
       </c>
       <c r="C116">
-        <v>27.1</v>
+        <v>15.1</v>
       </c>
       <c r="D116">
-        <v>28.1</v>
+        <v>15.6</v>
       </c>
       <c r="E116">
-        <v>31</v>
+        <v>17.3</v>
       </c>
       <c r="F116">
-        <v>27.06</v>
+        <v>15.06</v>
       </c>
       <c r="G116">
-        <v>3.99</v>
+        <v>0.2</v>
       </c>
       <c r="H116">
         <v>1801108.2</v>
@@ -6159,19 +6159,19 @@
         </is>
       </c>
       <c r="B117">
-        <v>120.6</v>
+        <v>109.7</v>
       </c>
       <c r="C117">
-        <v>115.4</v>
+        <v>105</v>
       </c>
       <c r="D117">
+        <v>107.4</v>
+      </c>
+      <c r="E117">
         <v>118</v>
       </c>
-      <c r="E117">
-        <v>129.7</v>
-      </c>
       <c r="F117">
-        <v>115.43</v>
+        <v>105</v>
       </c>
       <c r="G117">
         <v>0</v>
@@ -6192,22 +6192,22 @@
         </is>
       </c>
       <c r="B118">
-        <v>119.3</v>
+        <v>108.6</v>
       </c>
       <c r="C118">
-        <v>113.8</v>
+        <v>103.5</v>
       </c>
       <c r="D118">
-        <v>116.3</v>
+        <v>105.8</v>
       </c>
       <c r="E118">
-        <v>129.6</v>
+        <v>117.9</v>
       </c>
       <c r="F118">
-        <v>113.77</v>
+        <v>103.49</v>
       </c>
       <c r="G118">
-        <v>-1.66</v>
+        <v>-1.51</v>
       </c>
       <c r="H118">
         <v>3887490.3</v>
@@ -6225,22 +6225,22 @@
         </is>
       </c>
       <c r="B119">
-        <v>122.5</v>
+        <v>111.4</v>
       </c>
       <c r="C119">
-        <v>117.3</v>
+        <v>106.7</v>
       </c>
       <c r="D119">
-        <v>119.9</v>
+        <v>109.1</v>
       </c>
       <c r="E119">
-        <v>132.1</v>
+        <v>120.1</v>
       </c>
       <c r="F119">
-        <v>117.29</v>
+        <v>106.69</v>
       </c>
       <c r="G119">
-        <v>1.86</v>
+        <v>1.69</v>
       </c>
       <c r="H119">
         <v>4021362.4</v>
@@ -6258,22 +6258,22 @@
         </is>
       </c>
       <c r="B120">
-        <v>119.1</v>
+        <v>108.4</v>
       </c>
       <c r="C120">
-        <v>114.1</v>
+        <v>103.8</v>
       </c>
       <c r="D120">
+        <v>106.1</v>
+      </c>
+      <c r="E120">
         <v>116.7</v>
       </c>
-      <c r="E120">
-        <v>128.3</v>
-      </c>
       <c r="F120">
-        <v>114.09</v>
+        <v>103.78</v>
       </c>
       <c r="G120">
-        <v>-1.34</v>
+        <v>-1.22</v>
       </c>
       <c r="H120">
         <v>3877753.2</v>
@@ -6291,22 +6291,22 @@
         </is>
       </c>
       <c r="B121">
-        <v>118.9</v>
+        <v>108.2</v>
       </c>
       <c r="C121">
-        <v>114</v>
+        <v>103.7</v>
       </c>
       <c r="D121">
+        <v>105.9</v>
+      </c>
+      <c r="E121">
         <v>116.4</v>
       </c>
-      <c r="E121">
-        <v>127.9</v>
-      </c>
       <c r="F121">
-        <v>113.97</v>
+        <v>103.67</v>
       </c>
       <c r="G121">
-        <v>-1.46</v>
+        <v>-1.33</v>
       </c>
       <c r="H121">
         <v>4230178.7</v>
@@ -6324,19 +6324,19 @@
         </is>
       </c>
       <c r="B122">
-        <v>50.7</v>
+        <v>34.1</v>
       </c>
       <c r="C122">
-        <v>48.6</v>
+        <v>32.8</v>
       </c>
       <c r="D122">
-        <v>49.9</v>
+        <v>33.6</v>
       </c>
       <c r="E122">
-        <v>53.7</v>
+        <v>36.2</v>
       </c>
       <c r="F122">
-        <v>48.62</v>
+        <v>32.75</v>
       </c>
       <c r="G122">
         <v>0</v>
@@ -6357,22 +6357,22 @@
         </is>
       </c>
       <c r="B123">
-        <v>50.6</v>
+        <v>34.1</v>
       </c>
       <c r="C123">
-        <v>48.2</v>
+        <v>32.5</v>
       </c>
       <c r="D123">
-        <v>49.5</v>
+        <v>33.3</v>
       </c>
       <c r="E123">
-        <v>54.1</v>
+        <v>36.5</v>
       </c>
       <c r="F123">
-        <v>48.25</v>
+        <v>32.5</v>
       </c>
       <c r="G123">
-        <v>-0.37</v>
+        <v>-0.25</v>
       </c>
       <c r="H123">
         <v>216696.6</v>
@@ -6390,22 +6390,22 @@
         </is>
       </c>
       <c r="B124">
-        <v>58.4</v>
+        <v>39.4</v>
       </c>
       <c r="C124">
-        <v>56</v>
+        <v>37.7</v>
       </c>
       <c r="D124">
-        <v>57.4</v>
+        <v>38.7</v>
       </c>
       <c r="E124">
-        <v>61.9</v>
+        <v>41.7</v>
       </c>
       <c r="F124">
-        <v>55.98</v>
+        <v>37.71</v>
       </c>
       <c r="G124">
-        <v>7.36</v>
+        <v>4.96</v>
       </c>
       <c r="H124">
         <v>329309</v>
@@ -6423,22 +6423,22 @@
         </is>
       </c>
       <c r="B125">
-        <v>49.9</v>
+        <v>33.6</v>
       </c>
       <c r="C125">
-        <v>47.9</v>
+        <v>32.2</v>
       </c>
       <c r="D125">
-        <v>49.1</v>
+        <v>33.1</v>
       </c>
       <c r="E125">
-        <v>52.9</v>
+        <v>35.6</v>
       </c>
       <c r="F125">
-        <v>47.85</v>
+        <v>32.23</v>
       </c>
       <c r="G125">
-        <v>-0.77</v>
+        <v>-0.52</v>
       </c>
       <c r="H125">
         <v>205882.4</v>
@@ -6456,22 +6456,22 @@
         </is>
       </c>
       <c r="B126">
-        <v>50.4</v>
+        <v>34</v>
       </c>
       <c r="C126">
-        <v>48.4</v>
+        <v>32.6</v>
       </c>
       <c r="D126">
-        <v>49.6</v>
+        <v>33.4</v>
       </c>
       <c r="E126">
-        <v>53.3</v>
+        <v>35.9</v>
       </c>
       <c r="F126">
-        <v>48.36</v>
+        <v>32.58</v>
       </c>
       <c r="G126">
-        <v>-0.26</v>
+        <v>-0.17</v>
       </c>
       <c r="H126">
         <v>236087.9</v>
@@ -6819,19 +6819,19 @@
         </is>
       </c>
       <c r="B137">
-        <v>10</v>
+        <v>14.7</v>
       </c>
       <c r="C137">
-        <v>9.5</v>
+        <v>14</v>
       </c>
       <c r="D137">
-        <v>9.800000000000001</v>
+        <v>14.5</v>
       </c>
       <c r="E137">
-        <v>10.6</v>
+        <v>15.5</v>
       </c>
       <c r="F137">
-        <v>9.52</v>
+        <v>14</v>
       </c>
       <c r="G137">
         <v>0</v>
@@ -6852,22 +6852,22 @@
         </is>
       </c>
       <c r="B138">
-        <v>10</v>
+        <v>14.7</v>
       </c>
       <c r="C138">
-        <v>9.5</v>
+        <v>13.9</v>
       </c>
       <c r="D138">
-        <v>9.800000000000001</v>
+        <v>14.5</v>
       </c>
       <c r="E138">
-        <v>10.7</v>
+        <v>15.7</v>
       </c>
       <c r="F138">
-        <v>9.470000000000001</v>
+        <v>13.93</v>
       </c>
       <c r="G138">
-        <v>-0.05</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H138">
         <v>403826.3</v>
@@ -6885,22 +6885,22 @@
         </is>
       </c>
       <c r="B139">
-        <v>10.4</v>
+        <v>15.3</v>
       </c>
       <c r="C139">
-        <v>9.9</v>
+        <v>14.6</v>
       </c>
       <c r="D139">
-        <v>10.3</v>
+        <v>15.1</v>
       </c>
       <c r="E139">
-        <v>11</v>
+        <v>16.1</v>
       </c>
       <c r="F139">
-        <v>9.93</v>
+        <v>14.6</v>
       </c>
       <c r="G139">
-        <v>0.41</v>
+        <v>0.6</v>
       </c>
       <c r="H139">
         <v>488705.3</v>
@@ -6918,22 +6918,22 @@
         </is>
       </c>
       <c r="B140">
-        <v>9.699999999999999</v>
+        <v>14.2</v>
       </c>
       <c r="C140">
-        <v>9.300000000000001</v>
+        <v>13.6</v>
       </c>
       <c r="D140">
-        <v>9.6</v>
+        <v>14.1</v>
       </c>
       <c r="E140">
-        <v>10.2</v>
+        <v>15</v>
       </c>
       <c r="F140">
-        <v>9.26</v>
+        <v>13.62</v>
       </c>
       <c r="G140">
-        <v>-0.26</v>
+        <v>-0.38</v>
       </c>
       <c r="H140">
         <v>364011</v>
@@ -6951,22 +6951,22 @@
         </is>
       </c>
       <c r="B141">
-        <v>9.699999999999999</v>
+        <v>14.3</v>
       </c>
       <c r="C141">
-        <v>9.300000000000001</v>
+        <v>13.7</v>
       </c>
       <c r="D141">
-        <v>9.6</v>
+        <v>14.2</v>
       </c>
       <c r="E141">
-        <v>10.3</v>
+        <v>15.1</v>
       </c>
       <c r="F141">
-        <v>9.31</v>
+        <v>13.7</v>
       </c>
       <c r="G141">
-        <v>-0.21</v>
+        <v>-0.3</v>
       </c>
       <c r="H141">
         <v>376302.1</v>

</xml_diff>

<commit_message>
Regen using V20 input params
</commit_message>
<xml_diff>
--- a/results/multi_city/AP/desc_stats.xlsx
+++ b/results/multi_city/AP/desc_stats.xlsx
@@ -2964,7 +2964,7 @@
         <v>24</v>
       </c>
       <c r="D20">
-        <v>26.3</v>
+        <v>26.4</v>
       </c>
       <c r="E20">
         <v>29.8</v>
@@ -3651,7 +3651,7 @@
         </is>
       </c>
       <c r="B41">
-        <v>14.8</v>
+        <v>14.7</v>
       </c>
       <c r="C41">
         <v>13.7</v>
@@ -4152,7 +4152,7 @@
         <v>20.9</v>
       </c>
       <c r="D56">
-        <v>22.1</v>
+        <v>22</v>
       </c>
       <c r="E56">
         <v>23.6</v>
@@ -4584,7 +4584,7 @@
         <v>40.9</v>
       </c>
       <c r="E69">
-        <v>43.9</v>
+        <v>43.8</v>
       </c>
       <c r="F69">
         <v>38.45</v>
@@ -4650,7 +4650,7 @@
         <v>40</v>
       </c>
       <c r="E71">
-        <v>42.9</v>
+        <v>42.8</v>
       </c>
       <c r="F71">
         <v>37.65</v>
@@ -4845,7 +4845,7 @@
         <v>21.9</v>
       </c>
       <c r="D77">
-        <v>23</v>
+        <v>22.9</v>
       </c>
       <c r="E77">
         <v>24.9</v>
@@ -5598,7 +5598,7 @@
         </is>
       </c>
       <c r="B100">
-        <v>36.5</v>
+        <v>36.4</v>
       </c>
       <c r="C100">
         <v>34.2</v>
@@ -5670,7 +5670,7 @@
         <v>55</v>
       </c>
       <c r="D102">
-        <v>59.3</v>
+        <v>59.2</v>
       </c>
       <c r="E102">
         <v>65.40000000000001</v>
@@ -5796,13 +5796,13 @@
         </is>
       </c>
       <c r="B106">
-        <v>59.6</v>
+        <v>59.7</v>
       </c>
       <c r="C106">
         <v>54.4</v>
       </c>
       <c r="D106">
-        <v>58.5</v>
+        <v>58.6</v>
       </c>
       <c r="E106">
         <v>64.7</v>
@@ -6168,7 +6168,7 @@
         <v>107.4</v>
       </c>
       <c r="E117">
-        <v>118</v>
+        <v>118.1</v>
       </c>
       <c r="F117">
         <v>105</v>
@@ -6234,7 +6234,7 @@
         <v>109.1</v>
       </c>
       <c r="E119">
-        <v>120.1</v>
+        <v>120.2</v>
       </c>
       <c r="F119">
         <v>106.69</v>
@@ -6267,7 +6267,7 @@
         <v>106.1</v>
       </c>
       <c r="E120">
-        <v>116.6</v>
+        <v>116.8</v>
       </c>
       <c r="F120">
         <v>103.78</v>
@@ -6432,7 +6432,7 @@
         <v>33.1</v>
       </c>
       <c r="E125">
-        <v>35.6</v>
+        <v>35.7</v>
       </c>
       <c r="F125">
         <v>32.23</v>

</xml_diff>

<commit_message>
Regen results folder using v24 of InputParams
</commit_message>
<xml_diff>
--- a/results/multi_city/AP/desc_stats.xlsx
+++ b/results/multi_city/AP/desc_stats.xlsx
@@ -1940,13 +1940,13 @@
         </is>
       </c>
       <c r="B3">
-        <v>48409.4</v>
+        <v>48414.1</v>
       </c>
       <c r="C3">
-        <v>44488.6</v>
+        <v>44487.2</v>
       </c>
       <c r="D3">
-        <v>588061</v>
+        <v>587390.8</v>
       </c>
       <c r="E3">
         <v>1550837</v>
@@ -1955,73 +1955,73 @@
         <v>2964297.1</v>
       </c>
       <c r="G3">
-        <v>499058.9</v>
+        <v>499054.8</v>
       </c>
       <c r="H3">
         <v>5126.4</v>
       </c>
       <c r="I3">
-        <v>31585.7</v>
+        <v>31542.1</v>
       </c>
       <c r="J3">
-        <v>1142880.7</v>
+        <v>1142859</v>
       </c>
       <c r="K3">
-        <v>48338.1</v>
+        <v>48335.4</v>
       </c>
       <c r="L3">
-        <v>487813</v>
+        <v>487784.7</v>
       </c>
       <c r="M3">
-        <v>3264384.2</v>
+        <v>3264287.9</v>
       </c>
       <c r="N3">
-        <v>293981.3</v>
+        <v>293964.3</v>
       </c>
       <c r="O3">
-        <v>26655.9</v>
+        <v>26651.9</v>
       </c>
       <c r="P3">
-        <v>80097.3</v>
+        <v>79985.60000000001</v>
       </c>
       <c r="Q3">
-        <v>59392.8</v>
+        <v>59397</v>
       </c>
       <c r="R3">
-        <v>417539.7</v>
+        <v>417495.2</v>
       </c>
       <c r="S3">
         <v>2722312.2</v>
       </c>
       <c r="T3">
-        <v>8888.6</v>
+        <v>8888</v>
       </c>
       <c r="U3">
-        <v>8574.700000000001</v>
+        <v>8574.1</v>
       </c>
       <c r="V3">
         <v>388200.1</v>
       </c>
       <c r="W3">
-        <v>2117283.2</v>
+        <v>2117441.3</v>
       </c>
       <c r="X3">
-        <v>1749135.7</v>
+        <v>1748485.7</v>
       </c>
       <c r="Y3">
-        <v>3887490.3</v>
+        <v>3885930.4</v>
       </c>
       <c r="Z3">
-        <v>216696.6</v>
+        <v>217618.6</v>
       </c>
       <c r="AA3">
-        <v>6835.1</v>
+        <v>6834.4</v>
       </c>
       <c r="AB3">
-        <v>494736.8</v>
+        <v>494683.9</v>
       </c>
       <c r="AC3">
-        <v>403826.3</v>
+        <v>403289.8</v>
       </c>
     </row>
     <row r="4">
@@ -2031,13 +2031,13 @@
         </is>
       </c>
       <c r="B4">
-        <v>51988</v>
+        <v>51977.2</v>
       </c>
       <c r="C4">
-        <v>50433.2</v>
+        <v>50418.8</v>
       </c>
       <c r="D4">
-        <v>622456.7</v>
+        <v>620064.1</v>
       </c>
       <c r="E4">
         <v>1756205.4</v>
@@ -2046,73 +2046,73 @@
         <v>3606770.2</v>
       </c>
       <c r="G4">
-        <v>592904.4</v>
+        <v>578540.6</v>
       </c>
       <c r="H4">
-        <v>5450.6</v>
+        <v>5449.8</v>
       </c>
       <c r="I4">
-        <v>35052.2</v>
+        <v>35065.2</v>
       </c>
       <c r="J4">
-        <v>1223128.4</v>
+        <v>1222888.1</v>
       </c>
       <c r="K4">
-        <v>51905</v>
+        <v>51895.2</v>
       </c>
       <c r="L4">
-        <v>634328.2</v>
+        <v>610751.9</v>
       </c>
       <c r="M4">
-        <v>3710629.8</v>
+        <v>3707770.6</v>
       </c>
       <c r="N4">
-        <v>342033.7</v>
+        <v>341094.4</v>
       </c>
       <c r="O4">
-        <v>28101.8</v>
+        <v>28101.3</v>
       </c>
       <c r="P4">
-        <v>86847.60000000001</v>
+        <v>87167.10000000001</v>
       </c>
       <c r="Q4">
-        <v>63873.9</v>
+        <v>63834.8</v>
       </c>
       <c r="R4">
-        <v>456914.8</v>
+        <v>456489.4</v>
       </c>
       <c r="S4">
         <v>2957194.8</v>
       </c>
       <c r="T4">
-        <v>9222.200000000001</v>
+        <v>9232.1</v>
       </c>
       <c r="U4">
-        <v>8865.9</v>
+        <v>8865.6</v>
       </c>
       <c r="V4">
         <v>487932.1</v>
       </c>
       <c r="W4">
-        <v>2628058.3</v>
+        <v>2694343.8</v>
       </c>
       <c r="X4">
-        <v>1817428.1</v>
+        <v>1818676.7</v>
       </c>
       <c r="Y4">
-        <v>4021362.4</v>
+        <v>4040523.4</v>
       </c>
       <c r="Z4">
-        <v>329309</v>
+        <v>335537.3</v>
       </c>
       <c r="AA4">
-        <v>8978.799999999999</v>
+        <v>9399.700000000001</v>
       </c>
       <c r="AB4">
-        <v>565927.3</v>
+        <v>570903.9</v>
       </c>
       <c r="AC4">
-        <v>488705.3</v>
+        <v>500335.8</v>
       </c>
     </row>
     <row r="5">
@@ -2122,13 +2122,13 @@
         </is>
       </c>
       <c r="B5">
-        <v>46125</v>
+        <v>46124.8</v>
       </c>
       <c r="C5">
-        <v>42304.9</v>
+        <v>42308.8</v>
       </c>
       <c r="D5">
-        <v>564328.1</v>
+        <v>563626.8</v>
       </c>
       <c r="E5">
         <v>1433623.7</v>
@@ -2137,73 +2137,73 @@
         <v>2533020.5</v>
       </c>
       <c r="G5">
-        <v>480621.6</v>
+        <v>478203.9</v>
       </c>
       <c r="H5">
-        <v>4980.4</v>
+        <v>4980.2</v>
       </c>
       <c r="I5">
-        <v>29247.4</v>
+        <v>29255.8</v>
       </c>
       <c r="J5">
-        <v>1084665.1</v>
+        <v>1084843.3</v>
       </c>
       <c r="K5">
-        <v>46630.2</v>
+        <v>46635.5</v>
       </c>
       <c r="L5">
-        <v>466646.9</v>
+        <v>464144.9</v>
       </c>
       <c r="M5">
-        <v>2968718.8</v>
+        <v>2968397.2</v>
       </c>
       <c r="N5">
-        <v>262130.9</v>
+        <v>262014.5</v>
       </c>
       <c r="O5">
-        <v>26165</v>
+        <v>26164.4</v>
       </c>
       <c r="P5">
-        <v>77037.7</v>
+        <v>76880</v>
       </c>
       <c r="Q5">
-        <v>57382.6</v>
+        <v>57355.5</v>
       </c>
       <c r="R5">
-        <v>396212.3</v>
+        <v>396086.4</v>
       </c>
       <c r="S5">
         <v>2542699.8</v>
       </c>
       <c r="T5">
-        <v>8667.6</v>
+        <v>8677.299999999999</v>
       </c>
       <c r="U5">
-        <v>8430.1</v>
+        <v>8431</v>
       </c>
       <c r="V5">
         <v>343146.4</v>
       </c>
       <c r="W5">
-        <v>2108705.5</v>
+        <v>2119750.7</v>
       </c>
       <c r="X5">
-        <v>1735620.8</v>
+        <v>1736083.1</v>
       </c>
       <c r="Y5">
-        <v>3877753.2</v>
+        <v>3909321.5</v>
       </c>
       <c r="Z5">
-        <v>205882.4</v>
+        <v>206331.1</v>
       </c>
       <c r="AA5">
-        <v>6360.9</v>
+        <v>6445.5</v>
       </c>
       <c r="AB5">
-        <v>445130.4</v>
+        <v>445449</v>
       </c>
       <c r="AC5">
-        <v>364011</v>
+        <v>375481</v>
       </c>
     </row>
     <row r="6">
@@ -2213,13 +2213,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>58156.5</v>
+        <v>60203.8</v>
       </c>
       <c r="C6">
-        <v>54774.5</v>
+        <v>56929</v>
       </c>
       <c r="D6">
-        <v>631201.2</v>
+        <v>648651.4</v>
       </c>
       <c r="E6">
         <v>1513636.8</v>
@@ -2228,73 +2228,73 @@
         <v>2941384</v>
       </c>
       <c r="G6">
-        <v>479622.9</v>
+        <v>480003</v>
       </c>
       <c r="H6">
-        <v>5953.3</v>
+        <v>6131.2</v>
       </c>
       <c r="I6">
-        <v>42631.1</v>
+        <v>45077.8</v>
       </c>
       <c r="J6">
-        <v>1367110.9</v>
+        <v>1406225.4</v>
       </c>
       <c r="K6">
-        <v>58506.3</v>
+        <v>60683.8</v>
       </c>
       <c r="L6">
-        <v>475516.7</v>
+        <v>476418.3</v>
       </c>
       <c r="M6">
-        <v>3273917.1</v>
+        <v>3292816</v>
       </c>
       <c r="N6">
-        <v>283197.6</v>
+        <v>284404.7</v>
       </c>
       <c r="O6">
-        <v>29922.4</v>
+        <v>30612</v>
       </c>
       <c r="P6">
-        <v>132726.4</v>
+        <v>141011.4</v>
       </c>
       <c r="Q6">
-        <v>68182</v>
+        <v>69908</v>
       </c>
       <c r="R6">
-        <v>436490.2</v>
+        <v>449972</v>
       </c>
       <c r="S6">
         <v>3500739.2</v>
       </c>
       <c r="T6">
-        <v>9690.5</v>
+        <v>9850.299999999999</v>
       </c>
       <c r="U6">
-        <v>9306.4</v>
+        <v>9456.5</v>
       </c>
       <c r="V6">
         <v>384853.7</v>
       </c>
       <c r="W6">
-        <v>2093151.2</v>
+        <v>2084559.9</v>
       </c>
       <c r="X6">
-        <v>1801108.2</v>
+        <v>1764447.9</v>
       </c>
       <c r="Y6">
-        <v>4230178.7</v>
+        <v>4119062.6</v>
       </c>
       <c r="Z6">
-        <v>236087.9</v>
+        <v>232812</v>
       </c>
       <c r="AA6">
-        <v>6432.6</v>
+        <v>6259</v>
       </c>
       <c r="AB6">
-        <v>482002.2</v>
+        <v>480470.6</v>
       </c>
       <c r="AC6">
-        <v>376302.1</v>
+        <v>383645.5</v>
       </c>
     </row>
   </sheetData>
@@ -2415,7 +2415,7 @@
         <v>-0.1</v>
       </c>
       <c r="H3">
-        <v>48409.4</v>
+        <v>48414.1</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2448,7 +2448,7 @@
         <v>0.19</v>
       </c>
       <c r="H4">
-        <v>51988</v>
+        <v>51977.2</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2481,7 +2481,7 @@
         <v>-0.26</v>
       </c>
       <c r="H5">
-        <v>46125</v>
+        <v>46124.8</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2508,13 +2508,13 @@
         <v>11.8</v>
       </c>
       <c r="F6">
-        <v>10.4</v>
+        <v>10.41</v>
       </c>
       <c r="G6">
-        <v>-0.1</v>
+        <v>-0.08</v>
       </c>
       <c r="H6">
-        <v>58156.5</v>
+        <v>60203.8</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2580,7 +2580,7 @@
         <v>-0.2</v>
       </c>
       <c r="H8">
-        <v>44488.6</v>
+        <v>44487.2</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         <v>0.41</v>
       </c>
       <c r="H9">
-        <v>50433.2</v>
+        <v>50418.8</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -2646,7 +2646,7 @@
         <v>-0.37</v>
       </c>
       <c r="H10">
-        <v>42304.9</v>
+        <v>42308.8</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -2667,19 +2667,19 @@
         <v>12.4</v>
       </c>
       <c r="D11">
-        <v>13</v>
+        <v>13.1</v>
       </c>
       <c r="E11">
         <v>14</v>
       </c>
       <c r="F11">
-        <v>12.37</v>
+        <v>12.4</v>
       </c>
       <c r="G11">
-        <v>-0.19</v>
+        <v>-0.17</v>
       </c>
       <c r="H11">
-        <v>54774.5</v>
+        <v>56929</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -2745,7 +2745,7 @@
         <v>-0.08</v>
       </c>
       <c r="H13">
-        <v>588061</v>
+        <v>587390.8</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -2772,13 +2772,13 @@
         <v>19.8</v>
       </c>
       <c r="F14">
-        <v>17.3</v>
+        <v>17.29</v>
       </c>
       <c r="G14">
-        <v>0.3</v>
+        <v>0.29</v>
       </c>
       <c r="H14">
-        <v>622456.7</v>
+        <v>620064.1</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -2811,7 +2811,7 @@
         <v>-0.26</v>
       </c>
       <c r="H15">
-        <v>564328.1</v>
+        <v>563626.8</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -2838,13 +2838,13 @@
         <v>19.3</v>
       </c>
       <c r="F16">
-        <v>16.9</v>
+        <v>16.92</v>
       </c>
       <c r="G16">
-        <v>-0.1</v>
+        <v>-0.08</v>
       </c>
       <c r="H16">
-        <v>631201.2</v>
+        <v>648651.4</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -3240,7 +3240,7 @@
         <v>-0.15</v>
       </c>
       <c r="H28">
-        <v>499058.9</v>
+        <v>499054.8</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -3258,7 +3258,7 @@
         <v>25.9</v>
       </c>
       <c r="C29">
-        <v>24.1</v>
+        <v>24</v>
       </c>
       <c r="D29">
         <v>25.1</v>
@@ -3267,13 +3267,13 @@
         <v>28.1</v>
       </c>
       <c r="F29">
-        <v>24.07</v>
+        <v>24.04</v>
       </c>
       <c r="G29">
-        <v>0.02</v>
+        <v>-0.01</v>
       </c>
       <c r="H29">
-        <v>592904.4</v>
+        <v>578540.6</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -3288,25 +3288,25 @@
         </is>
       </c>
       <c r="B30">
-        <v>26.1</v>
+        <v>26</v>
       </c>
       <c r="C30">
-        <v>24.3</v>
+        <v>24.2</v>
       </c>
       <c r="D30">
-        <v>25.3</v>
+        <v>25.2</v>
       </c>
       <c r="E30">
-        <v>28.4</v>
+        <v>28.3</v>
       </c>
       <c r="F30">
-        <v>24.27</v>
+        <v>24.18</v>
       </c>
       <c r="G30">
-        <v>0.22</v>
+        <v>0.13</v>
       </c>
       <c r="H30">
-        <v>480621.6</v>
+        <v>478203.9</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -3339,7 +3339,7 @@
         <v>-0.26</v>
       </c>
       <c r="H31">
-        <v>479622.9</v>
+        <v>480003</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -3438,7 +3438,7 @@
         <v>0.22</v>
       </c>
       <c r="H34">
-        <v>5450.6</v>
+        <v>5449.8</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -3471,7 +3471,7 @@
         <v>-0.24</v>
       </c>
       <c r="H35">
-        <v>4980.4</v>
+        <v>4980.2</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -3498,13 +3498,13 @@
         <v>17.6</v>
       </c>
       <c r="F36">
-        <v>15.42</v>
+        <v>15.44</v>
       </c>
       <c r="G36">
-        <v>-0.19</v>
+        <v>-0.16</v>
       </c>
       <c r="H36">
-        <v>5953.3</v>
+        <v>6131.2</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -3567,10 +3567,10 @@
         <v>13.73</v>
       </c>
       <c r="G38">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H38">
-        <v>31585.7</v>
+        <v>31542.1</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -3594,16 +3594,16 @@
         <v>15.1</v>
       </c>
       <c r="E39">
-        <v>16.3</v>
+        <v>16.4</v>
       </c>
       <c r="F39">
-        <v>14.29</v>
+        <v>14.3</v>
       </c>
       <c r="G39">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="H39">
-        <v>35052.2</v>
+        <v>35065.2</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -3630,13 +3630,13 @@
         <v>15.3</v>
       </c>
       <c r="F40">
-        <v>13.42</v>
+        <v>13.4</v>
       </c>
       <c r="G40">
-        <v>-0.46</v>
+        <v>-0.48</v>
       </c>
       <c r="H40">
-        <v>29247.4</v>
+        <v>29255.8</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -3651,25 +3651,25 @@
         </is>
       </c>
       <c r="B41">
-        <v>14.7</v>
+        <v>14.8</v>
       </c>
       <c r="C41">
-        <v>13.7</v>
+        <v>13.8</v>
       </c>
       <c r="D41">
-        <v>14.5</v>
+        <v>14.6</v>
       </c>
       <c r="E41">
         <v>15.7</v>
       </c>
       <c r="F41">
-        <v>13.73</v>
+        <v>13.78</v>
       </c>
       <c r="G41">
-        <v>-0.15</v>
+        <v>-0.11</v>
       </c>
       <c r="H41">
-        <v>42631.1</v>
+        <v>45077.8</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -3735,7 +3735,7 @@
         <v>-0.14</v>
       </c>
       <c r="H43">
-        <v>1142880.7</v>
+        <v>1142859</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -3768,7 +3768,7 @@
         <v>0.28</v>
       </c>
       <c r="H44">
-        <v>1223128.4</v>
+        <v>1222888.1</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -3801,7 +3801,7 @@
         <v>-0.35</v>
       </c>
       <c r="H45">
-        <v>1084665.1</v>
+        <v>1084843.3</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -3828,13 +3828,13 @@
         <v>17.1</v>
       </c>
       <c r="F46">
-        <v>14.97</v>
+        <v>14.99</v>
       </c>
       <c r="G46">
-        <v>-0.12</v>
+        <v>-0.1</v>
       </c>
       <c r="H46">
-        <v>1367110.9</v>
+        <v>1406225.4</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -3900,7 +3900,7 @@
         <v>-0.12</v>
       </c>
       <c r="H48">
-        <v>48338.1</v>
+        <v>48335.4</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -3933,7 +3933,7 @@
         <v>0.2</v>
       </c>
       <c r="H49">
-        <v>51905</v>
+        <v>51895.2</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -3966,7 +3966,7 @@
         <v>-0.23</v>
       </c>
       <c r="H50">
-        <v>46630.2</v>
+        <v>46635.5</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -3981,25 +3981,25 @@
         </is>
       </c>
       <c r="B51">
-        <v>12.2</v>
+        <v>12.3</v>
       </c>
       <c r="C51">
         <v>11.6</v>
       </c>
       <c r="D51">
-        <v>12.1</v>
+        <v>12.2</v>
       </c>
       <c r="E51">
         <v>13</v>
       </c>
       <c r="F51">
-        <v>11.55</v>
+        <v>11.57</v>
       </c>
       <c r="G51">
-        <v>-0.13</v>
+        <v>-0.11</v>
       </c>
       <c r="H51">
-        <v>58506.3</v>
+        <v>60683.8</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -4065,7 +4065,7 @@
         <v>-0.14</v>
       </c>
       <c r="H53">
-        <v>487813</v>
+        <v>487784.7</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -4080,25 +4080,25 @@
         </is>
       </c>
       <c r="B54">
-        <v>22.6</v>
+        <v>22.5</v>
       </c>
       <c r="C54">
-        <v>21.2</v>
+        <v>21.1</v>
       </c>
       <c r="D54">
         <v>22.4</v>
       </c>
       <c r="E54">
-        <v>24.2</v>
+        <v>24.1</v>
       </c>
       <c r="F54">
-        <v>21.17</v>
+        <v>21.13</v>
       </c>
       <c r="G54">
-        <v>0.08</v>
+        <v>0.04</v>
       </c>
       <c r="H54">
-        <v>634328.2</v>
+        <v>610751.9</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
@@ -4113,25 +4113,25 @@
         </is>
       </c>
       <c r="B55">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="C55">
-        <v>21.3</v>
+        <v>21.2</v>
       </c>
       <c r="D55">
-        <v>22.6</v>
+        <v>22.5</v>
       </c>
       <c r="E55">
-        <v>24.2</v>
+        <v>24.1</v>
       </c>
       <c r="F55">
-        <v>21.28</v>
+        <v>21.21</v>
       </c>
       <c r="G55">
-        <v>0.19</v>
+        <v>0.12</v>
       </c>
       <c r="H55">
-        <v>466646.9</v>
+        <v>464144.9</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -4164,7 +4164,7 @@
         <v>-0.2</v>
       </c>
       <c r="H56">
-        <v>475516.7</v>
+        <v>476418.3</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -4230,7 +4230,7 @@
         <v>-0.21</v>
       </c>
       <c r="H58">
-        <v>3264384.2</v>
+        <v>3264287.9</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -4248,7 +4248,7 @@
         <v>55.8</v>
       </c>
       <c r="C59">
-        <v>51.3</v>
+        <v>51.2</v>
       </c>
       <c r="D59">
         <v>55.2</v>
@@ -4257,13 +4257,13 @@
         <v>60.4</v>
       </c>
       <c r="F59">
-        <v>51.25</v>
+        <v>51.24</v>
       </c>
       <c r="G59">
-        <v>1.25</v>
+        <v>1.24</v>
       </c>
       <c r="H59">
-        <v>3710629.8</v>
+        <v>3707770.6</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
@@ -4296,7 +4296,7 @@
         <v>-1.27</v>
       </c>
       <c r="H60">
-        <v>2968718.8</v>
+        <v>2968397.2</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -4311,25 +4311,25 @@
         </is>
       </c>
       <c r="B61">
-        <v>54.6</v>
+        <v>54.7</v>
       </c>
       <c r="C61">
-        <v>50.2</v>
+        <v>50.3</v>
       </c>
       <c r="D61">
-        <v>54</v>
+        <v>54.1</v>
       </c>
       <c r="E61">
-        <v>58.9</v>
+        <v>59</v>
       </c>
       <c r="F61">
-        <v>50.19</v>
+        <v>50.33</v>
       </c>
       <c r="G61">
-        <v>0.19</v>
+        <v>0.33</v>
       </c>
       <c r="H61">
-        <v>3273917.1</v>
+        <v>3292816</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
@@ -4395,7 +4395,7 @@
         <v>-0.1</v>
       </c>
       <c r="H63">
-        <v>293981.3</v>
+        <v>293964.3</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -4422,13 +4422,13 @@
         <v>17.9</v>
       </c>
       <c r="F64">
-        <v>15.55</v>
+        <v>15.54</v>
       </c>
       <c r="G64">
         <v>-0.03</v>
       </c>
       <c r="H64">
-        <v>342033.7</v>
+        <v>341094.4</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
@@ -4455,13 +4455,13 @@
         <v>17.9</v>
       </c>
       <c r="F65">
-        <v>15.52</v>
+        <v>15.51</v>
       </c>
       <c r="G65">
         <v>-0.06</v>
       </c>
       <c r="H65">
-        <v>262130.9</v>
+        <v>262014.5</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -4491,10 +4491,10 @@
         <v>15.43</v>
       </c>
       <c r="G66">
-        <v>-0.15</v>
+        <v>-0.14</v>
       </c>
       <c r="H66">
-        <v>283197.6</v>
+        <v>284404.7</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -4560,7 +4560,7 @@
         <v>-0.43</v>
       </c>
       <c r="H68">
-        <v>26655.9</v>
+        <v>26651.9</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -4590,10 +4590,10 @@
         <v>38.45</v>
       </c>
       <c r="G69">
-        <v>0.36</v>
+        <v>0.35</v>
       </c>
       <c r="H69">
-        <v>28101.8</v>
+        <v>28101.3</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
@@ -4626,7 +4626,7 @@
         <v>-0.53</v>
       </c>
       <c r="H70">
-        <v>26165</v>
+        <v>26164.4</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
@@ -4641,7 +4641,7 @@
         </is>
       </c>
       <c r="B71">
-        <v>40.2</v>
+        <v>40.3</v>
       </c>
       <c r="C71">
         <v>37.7</v>
@@ -4650,16 +4650,16 @@
         <v>40</v>
       </c>
       <c r="E71">
-        <v>42.8</v>
+        <v>42.9</v>
       </c>
       <c r="F71">
-        <v>37.65</v>
+        <v>37.69</v>
       </c>
       <c r="G71">
-        <v>-0.45</v>
+        <v>-0.4</v>
       </c>
       <c r="H71">
-        <v>29922.4</v>
+        <v>30612</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
@@ -4716,16 +4716,16 @@
         <v>28.1</v>
       </c>
       <c r="E73">
-        <v>30.9</v>
+        <v>30.8</v>
       </c>
       <c r="F73">
-        <v>26.07</v>
+        <v>26.06</v>
       </c>
       <c r="G73">
         <v>-0.25</v>
       </c>
       <c r="H73">
-        <v>80097.3</v>
+        <v>79985.60000000001</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
@@ -4752,13 +4752,13 @@
         <v>31.3</v>
       </c>
       <c r="F74">
-        <v>26.9</v>
+        <v>26.91</v>
       </c>
       <c r="G74">
-        <v>0.58</v>
+        <v>0.59</v>
       </c>
       <c r="H74">
-        <v>86847.60000000001</v>
+        <v>87167.10000000001</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
@@ -4791,7 +4791,7 @@
         <v>-0.55</v>
       </c>
       <c r="H75">
-        <v>77037.7</v>
+        <v>76880</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
@@ -4806,25 +4806,25 @@
         </is>
       </c>
       <c r="B76">
-        <v>28.8</v>
+        <v>28.9</v>
       </c>
       <c r="C76">
-        <v>26.6</v>
+        <v>26.7</v>
       </c>
       <c r="D76">
-        <v>28.5</v>
+        <v>28.6</v>
       </c>
       <c r="E76">
-        <v>30.9</v>
+        <v>31</v>
       </c>
       <c r="F76">
-        <v>26.62</v>
+        <v>26.73</v>
       </c>
       <c r="G76">
-        <v>0.3</v>
+        <v>0.41</v>
       </c>
       <c r="H76">
-        <v>132726.4</v>
+        <v>141011.4</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
@@ -4890,7 +4890,7 @@
         <v>-0.24</v>
       </c>
       <c r="H78">
-        <v>59392.8</v>
+        <v>59397</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
@@ -4914,7 +4914,7 @@
         <v>23.4</v>
       </c>
       <c r="E79">
-        <v>25.4</v>
+        <v>25.3</v>
       </c>
       <c r="F79">
         <v>22.26</v>
@@ -4923,7 +4923,7 @@
         <v>0.4</v>
       </c>
       <c r="H79">
-        <v>63873.9</v>
+        <v>63834.8</v>
       </c>
       <c r="I79" t="inlineStr">
         <is>
@@ -4956,7 +4956,7 @@
         <v>-0.3</v>
       </c>
       <c r="H80">
-        <v>57382.6</v>
+        <v>57355.5</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
@@ -4977,19 +4977,19 @@
         <v>21.5</v>
       </c>
       <c r="D81">
-        <v>22.5</v>
+        <v>22.6</v>
       </c>
       <c r="E81">
         <v>24.4</v>
       </c>
       <c r="F81">
-        <v>21.5</v>
+        <v>21.53</v>
       </c>
       <c r="G81">
-        <v>-0.36</v>
+        <v>-0.33</v>
       </c>
       <c r="H81">
-        <v>68182</v>
+        <v>69908</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -5055,7 +5055,7 @@
         <v>-0.26</v>
       </c>
       <c r="H83">
-        <v>417539.7</v>
+        <v>417495.2</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
@@ -5082,13 +5082,13 @@
         <v>36</v>
       </c>
       <c r="F84">
-        <v>32.97</v>
+        <v>32.95</v>
       </c>
       <c r="G84">
-        <v>0.97</v>
+        <v>0.95</v>
       </c>
       <c r="H84">
-        <v>456914.8</v>
+        <v>456489.4</v>
       </c>
       <c r="I84" t="inlineStr">
         <is>
@@ -5115,13 +5115,13 @@
         <v>34</v>
       </c>
       <c r="F85">
-        <v>31.21</v>
+        <v>31.2</v>
       </c>
       <c r="G85">
-        <v>-0.79</v>
+        <v>-0.8</v>
       </c>
       <c r="H85">
-        <v>396212.3</v>
+        <v>396086.4</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
@@ -5142,19 +5142,19 @@
         <v>31.7</v>
       </c>
       <c r="D86">
-        <v>32.7</v>
+        <v>32.8</v>
       </c>
       <c r="E86">
-        <v>34.5</v>
+        <v>34.6</v>
       </c>
       <c r="F86">
-        <v>31.68</v>
+        <v>31.73</v>
       </c>
       <c r="G86">
-        <v>-0.32</v>
+        <v>-0.27</v>
       </c>
       <c r="H86">
-        <v>436490.2</v>
+        <v>449972</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -5385,7 +5385,7 @@
         <v>-0.34</v>
       </c>
       <c r="H93">
-        <v>8888.6</v>
+        <v>8888</v>
       </c>
       <c r="I93" t="inlineStr">
         <is>
@@ -5412,13 +5412,13 @@
         <v>36.8</v>
       </c>
       <c r="F94">
-        <v>32.06</v>
+        <v>32.07</v>
       </c>
       <c r="G94">
-        <v>0.16</v>
+        <v>0.18</v>
       </c>
       <c r="H94">
-        <v>9222.200000000001</v>
+        <v>9232.1</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -5448,10 +5448,10 @@
         <v>31.42</v>
       </c>
       <c r="G95">
-        <v>-0.47</v>
+        <v>-0.48</v>
       </c>
       <c r="H95">
-        <v>8667.6</v>
+        <v>8677.299999999999</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -5466,25 +5466,25 @@
         </is>
       </c>
       <c r="B96">
-        <v>33.8</v>
+        <v>33.9</v>
       </c>
       <c r="C96">
-        <v>31.5</v>
+        <v>31.6</v>
       </c>
       <c r="D96">
         <v>33.5</v>
       </c>
       <c r="E96">
-        <v>36.1</v>
+        <v>36.2</v>
       </c>
       <c r="F96">
-        <v>31.53</v>
+        <v>31.57</v>
       </c>
       <c r="G96">
-        <v>-0.37</v>
+        <v>-0.33</v>
       </c>
       <c r="H96">
-        <v>9690.5</v>
+        <v>9850.299999999999</v>
       </c>
       <c r="I96" t="inlineStr">
         <is>
@@ -5550,7 +5550,7 @@
         <v>-0.42</v>
       </c>
       <c r="H98">
-        <v>8574.700000000001</v>
+        <v>8574.1</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -5583,7 +5583,7 @@
         <v>0.08</v>
       </c>
       <c r="H99">
-        <v>8865.9</v>
+        <v>8865.6</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -5616,7 +5616,7 @@
         <v>-0.25</v>
       </c>
       <c r="H100">
-        <v>8430.1</v>
+        <v>8431</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
@@ -5634,22 +5634,22 @@
         <v>36.3</v>
       </c>
       <c r="C101">
-        <v>34</v>
+        <v>34.1</v>
       </c>
       <c r="D101">
-        <v>35.9</v>
+        <v>36</v>
       </c>
       <c r="E101">
         <v>38.5</v>
       </c>
       <c r="F101">
-        <v>34.03</v>
+        <v>34.06</v>
       </c>
       <c r="G101">
-        <v>-0.42</v>
+        <v>-0.39</v>
       </c>
       <c r="H101">
-        <v>9306.4</v>
+        <v>9456.5</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
@@ -5880,7 +5880,7 @@
         <v>-0.34</v>
       </c>
       <c r="H108">
-        <v>2117283.2</v>
+        <v>2117441.3</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -5895,25 +5895,25 @@
         </is>
       </c>
       <c r="B109">
-        <v>36.6</v>
+        <v>37.1</v>
       </c>
       <c r="C109">
-        <v>35.6</v>
+        <v>36.1</v>
       </c>
       <c r="D109">
-        <v>35.6</v>
+        <v>36.1</v>
       </c>
       <c r="E109">
-        <v>38.4</v>
+        <v>38.9</v>
       </c>
       <c r="F109">
-        <v>35.63</v>
+        <v>36.09</v>
       </c>
       <c r="G109">
-        <v>3.25</v>
+        <v>3.71</v>
       </c>
       <c r="H109">
-        <v>2628058.3</v>
+        <v>2694343.8</v>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -5928,25 +5928,25 @@
         </is>
       </c>
       <c r="B110">
-        <v>32.9</v>
+        <v>33</v>
       </c>
       <c r="C110">
-        <v>32</v>
+        <v>32.1</v>
       </c>
       <c r="D110">
-        <v>32</v>
+        <v>32.1</v>
       </c>
       <c r="E110">
         <v>34.5</v>
       </c>
       <c r="F110">
-        <v>32.03</v>
+        <v>32.09</v>
       </c>
       <c r="G110">
-        <v>-0.35</v>
+        <v>-0.29</v>
       </c>
       <c r="H110">
-        <v>2108705.5</v>
+        <v>2119750.7</v>
       </c>
       <c r="I110" t="inlineStr">
         <is>
@@ -5964,22 +5964,22 @@
         <v>32.4</v>
       </c>
       <c r="C111">
-        <v>31.6</v>
+        <v>31.5</v>
       </c>
       <c r="D111">
-        <v>31.6</v>
+        <v>31.5</v>
       </c>
       <c r="E111">
         <v>34</v>
       </c>
       <c r="F111">
-        <v>31.56</v>
+        <v>31.55</v>
       </c>
       <c r="G111">
-        <v>-0.82</v>
+        <v>-0.83</v>
       </c>
       <c r="H111">
-        <v>2093151.2</v>
+        <v>2084559.9</v>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -6039,13 +6039,13 @@
         <v>17.1</v>
       </c>
       <c r="F113">
-        <v>14.72</v>
+        <v>14.71</v>
       </c>
       <c r="G113">
-        <v>-0.14</v>
+        <v>-0.15</v>
       </c>
       <c r="H113">
-        <v>1749135.7</v>
+        <v>1748485.7</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -6060,25 +6060,25 @@
         </is>
       </c>
       <c r="B114">
-        <v>15.9</v>
+        <v>15.8</v>
       </c>
       <c r="C114">
         <v>14.8</v>
       </c>
       <c r="D114">
-        <v>15.4</v>
+        <v>15.3</v>
       </c>
       <c r="E114">
         <v>17</v>
       </c>
       <c r="F114">
-        <v>14.78</v>
+        <v>14.77</v>
       </c>
       <c r="G114">
-        <v>-0.08</v>
+        <v>-0.09</v>
       </c>
       <c r="H114">
-        <v>1817428.1</v>
+        <v>1818676.7</v>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -6111,7 +6111,7 @@
         <v>-0.03</v>
       </c>
       <c r="H115">
-        <v>1735620.8</v>
+        <v>1736083.1</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -6126,25 +6126,25 @@
         </is>
       </c>
       <c r="B116">
-        <v>16.1</v>
+        <v>15.9</v>
       </c>
       <c r="C116">
-        <v>15.1</v>
+        <v>14.9</v>
       </c>
       <c r="D116">
-        <v>15.6</v>
+        <v>15.5</v>
       </c>
       <c r="E116">
-        <v>17.3</v>
+        <v>17.1</v>
       </c>
       <c r="F116">
-        <v>15.06</v>
+        <v>14.88</v>
       </c>
       <c r="G116">
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="H116">
-        <v>1801108.2</v>
+        <v>1764447.9</v>
       </c>
       <c r="I116" t="inlineStr">
         <is>
@@ -6192,25 +6192,25 @@
         </is>
       </c>
       <c r="B118">
-        <v>108.6</v>
+        <v>108.5</v>
       </c>
       <c r="C118">
-        <v>103.5</v>
+        <v>103.4</v>
       </c>
       <c r="D118">
-        <v>105.8</v>
+        <v>105.7</v>
       </c>
       <c r="E118">
-        <v>118</v>
+        <v>117.6</v>
       </c>
       <c r="F118">
-        <v>103.49</v>
+        <v>103.41</v>
       </c>
       <c r="G118">
-        <v>-1.51</v>
+        <v>-1.59</v>
       </c>
       <c r="H118">
-        <v>3887490.3</v>
+        <v>3885930.4</v>
       </c>
       <c r="I118" t="inlineStr">
         <is>
@@ -6225,25 +6225,25 @@
         </is>
       </c>
       <c r="B119">
-        <v>111.5</v>
+        <v>111.8</v>
       </c>
       <c r="C119">
-        <v>106.7</v>
+        <v>107</v>
       </c>
       <c r="D119">
-        <v>109.1</v>
+        <v>109.4</v>
       </c>
       <c r="E119">
-        <v>120.2</v>
+        <v>120.4</v>
       </c>
       <c r="F119">
-        <v>106.69</v>
+        <v>107.04</v>
       </c>
       <c r="G119">
-        <v>1.69</v>
+        <v>2.04</v>
       </c>
       <c r="H119">
-        <v>4021362.4</v>
+        <v>4040523.4</v>
       </c>
       <c r="I119" t="inlineStr">
         <is>
@@ -6258,25 +6258,25 @@
         </is>
       </c>
       <c r="B120">
-        <v>108.4</v>
+        <v>108.5</v>
       </c>
       <c r="C120">
-        <v>103.8</v>
+        <v>103.9</v>
       </c>
       <c r="D120">
-        <v>106.1</v>
+        <v>106.2</v>
       </c>
       <c r="E120">
         <v>116.8</v>
       </c>
       <c r="F120">
-        <v>103.78</v>
+        <v>103.87</v>
       </c>
       <c r="G120">
-        <v>-1.22</v>
+        <v>-1.13</v>
       </c>
       <c r="H120">
-        <v>3877753.2</v>
+        <v>3909321.5</v>
       </c>
       <c r="I120" t="inlineStr">
         <is>
@@ -6291,25 +6291,25 @@
         </is>
       </c>
       <c r="B121">
-        <v>108.2</v>
+        <v>107.8</v>
       </c>
       <c r="C121">
-        <v>103.7</v>
+        <v>103.2</v>
       </c>
       <c r="D121">
-        <v>106</v>
+        <v>105.6</v>
       </c>
       <c r="E121">
-        <v>116.4</v>
+        <v>115.9</v>
       </c>
       <c r="F121">
-        <v>103.67</v>
+        <v>103.25</v>
       </c>
       <c r="G121">
-        <v>-1.33</v>
+        <v>-1.75</v>
       </c>
       <c r="H121">
-        <v>4230178.7</v>
+        <v>4119062.6</v>
       </c>
       <c r="I121" t="inlineStr">
         <is>
@@ -6363,19 +6363,19 @@
         <v>32.5</v>
       </c>
       <c r="D123">
-        <v>33.3</v>
+        <v>33.4</v>
       </c>
       <c r="E123">
         <v>36.5</v>
       </c>
       <c r="F123">
-        <v>32.5</v>
+        <v>32.53</v>
       </c>
       <c r="G123">
-        <v>-0.25</v>
+        <v>-0.22</v>
       </c>
       <c r="H123">
-        <v>216696.6</v>
+        <v>217618.6</v>
       </c>
       <c r="I123" t="inlineStr">
         <is>
@@ -6390,25 +6390,25 @@
         </is>
       </c>
       <c r="B124">
-        <v>39.4</v>
+        <v>39.7</v>
       </c>
       <c r="C124">
-        <v>37.7</v>
+        <v>38</v>
       </c>
       <c r="D124">
-        <v>38.7</v>
+        <v>39</v>
       </c>
       <c r="E124">
-        <v>41.7</v>
+        <v>42</v>
       </c>
       <c r="F124">
-        <v>37.71</v>
+        <v>37.98</v>
       </c>
       <c r="G124">
-        <v>4.96</v>
+        <v>5.23</v>
       </c>
       <c r="H124">
-        <v>329309</v>
+        <v>335537.3</v>
       </c>
       <c r="I124" t="inlineStr">
         <is>
@@ -6423,7 +6423,7 @@
         </is>
       </c>
       <c r="B125">
-        <v>33.7</v>
+        <v>33.6</v>
       </c>
       <c r="C125">
         <v>32.2</v>
@@ -6441,7 +6441,7 @@
         <v>-0.52</v>
       </c>
       <c r="H125">
-        <v>205882.4</v>
+        <v>206331.1</v>
       </c>
       <c r="I125" t="inlineStr">
         <is>
@@ -6462,19 +6462,19 @@
         <v>32.6</v>
       </c>
       <c r="D126">
-        <v>33.4</v>
+        <v>33.5</v>
       </c>
       <c r="E126">
-        <v>35.9</v>
+        <v>36</v>
       </c>
       <c r="F126">
-        <v>32.58</v>
+        <v>32.65</v>
       </c>
       <c r="G126">
-        <v>-0.17</v>
+        <v>-0.1</v>
       </c>
       <c r="H126">
-        <v>236087.9</v>
+        <v>232812</v>
       </c>
       <c r="I126" t="inlineStr">
         <is>
@@ -6540,7 +6540,7 @@
         <v>-0.06</v>
       </c>
       <c r="H128">
-        <v>6835.1</v>
+        <v>6834.4</v>
       </c>
       <c r="I128" t="inlineStr">
         <is>
@@ -6555,25 +6555,25 @@
         </is>
       </c>
       <c r="B129">
+        <v>12.1</v>
+      </c>
+      <c r="C129">
+        <v>11.6</v>
+      </c>
+      <c r="D129">
         <v>12</v>
       </c>
-      <c r="C129">
-        <v>11.5</v>
-      </c>
-      <c r="D129">
-        <v>11.8</v>
-      </c>
       <c r="E129">
-        <v>12.6</v>
+        <v>12.8</v>
       </c>
       <c r="F129">
-        <v>11.49</v>
+        <v>11.64</v>
       </c>
       <c r="G129">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="H129">
-        <v>8978.799999999999</v>
+        <v>9399.700000000001</v>
       </c>
       <c r="I129" t="inlineStr">
         <is>
@@ -6600,13 +6600,13 @@
         <v>11.6</v>
       </c>
       <c r="F130">
-        <v>10.56</v>
+        <v>10.59</v>
       </c>
       <c r="G130">
-        <v>-0.23</v>
+        <v>-0.2</v>
       </c>
       <c r="H130">
-        <v>6360.9</v>
+        <v>6445.5</v>
       </c>
       <c r="I130" t="inlineStr">
         <is>
@@ -6621,25 +6621,25 @@
         </is>
       </c>
       <c r="B131">
-        <v>11</v>
+        <v>10.9</v>
       </c>
       <c r="C131">
-        <v>10.6</v>
+        <v>10.5</v>
       </c>
       <c r="D131">
-        <v>10.9</v>
+        <v>10.8</v>
       </c>
       <c r="E131">
-        <v>11.6</v>
+        <v>11.5</v>
       </c>
       <c r="F131">
-        <v>10.58</v>
+        <v>10.52</v>
       </c>
       <c r="G131">
-        <v>-0.21</v>
+        <v>-0.27</v>
       </c>
       <c r="H131">
-        <v>6432.6</v>
+        <v>6259</v>
       </c>
       <c r="I131" t="inlineStr">
         <is>
@@ -6705,7 +6705,7 @@
         <v>-0.02</v>
       </c>
       <c r="H133">
-        <v>494736.8</v>
+        <v>494683.9</v>
       </c>
       <c r="I133" t="inlineStr">
         <is>
@@ -6732,13 +6732,13 @@
         <v>7.4</v>
       </c>
       <c r="F134">
-        <v>6.08</v>
+        <v>6.1</v>
       </c>
       <c r="G134">
-        <v>0.17</v>
+        <v>0.19</v>
       </c>
       <c r="H134">
-        <v>565927.3</v>
+        <v>570903.9</v>
       </c>
       <c r="I134" t="inlineStr">
         <is>
@@ -6771,7 +6771,7 @@
         <v>-0.15</v>
       </c>
       <c r="H135">
-        <v>445130.4</v>
+        <v>445449</v>
       </c>
       <c r="I135" t="inlineStr">
         <is>
@@ -6804,7 +6804,7 @@
         <v>-0.06</v>
       </c>
       <c r="H136">
-        <v>482002.2</v>
+        <v>480470.6</v>
       </c>
       <c r="I136" t="inlineStr">
         <is>
@@ -6864,13 +6864,13 @@
         <v>15.7</v>
       </c>
       <c r="F138">
-        <v>13.93</v>
+        <v>13.92</v>
       </c>
       <c r="G138">
-        <v>-0.07000000000000001</v>
+        <v>-0.08</v>
       </c>
       <c r="H138">
-        <v>403826.3</v>
+        <v>403289.8</v>
       </c>
       <c r="I138" t="inlineStr">
         <is>
@@ -6885,25 +6885,25 @@
         </is>
       </c>
       <c r="B139">
-        <v>15.3</v>
+        <v>15.4</v>
       </c>
       <c r="C139">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="D139">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="E139">
-        <v>16.2</v>
+        <v>16.3</v>
       </c>
       <c r="F139">
-        <v>14.6</v>
+        <v>14.7</v>
       </c>
       <c r="G139">
-        <v>0.6</v>
+        <v>0.7</v>
       </c>
       <c r="H139">
-        <v>488705.3</v>
+        <v>500335.8</v>
       </c>
       <c r="I139" t="inlineStr">
         <is>
@@ -6918,25 +6918,25 @@
         </is>
       </c>
       <c r="B140">
-        <v>14.3</v>
+        <v>14.4</v>
       </c>
       <c r="C140">
-        <v>13.6</v>
+        <v>13.7</v>
       </c>
       <c r="D140">
-        <v>14.1</v>
+        <v>14.2</v>
       </c>
       <c r="E140">
-        <v>15</v>
+        <v>15.1</v>
       </c>
       <c r="F140">
-        <v>13.62</v>
+        <v>13.71</v>
       </c>
       <c r="G140">
-        <v>-0.38</v>
+        <v>-0.29</v>
       </c>
       <c r="H140">
-        <v>364011</v>
+        <v>375481</v>
       </c>
       <c r="I140" t="inlineStr">
         <is>
@@ -6951,25 +6951,25 @@
         </is>
       </c>
       <c r="B141">
-        <v>14.3</v>
+        <v>14.4</v>
       </c>
       <c r="C141">
-        <v>13.7</v>
+        <v>13.8</v>
       </c>
       <c r="D141">
         <v>14.2</v>
       </c>
       <c r="E141">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="F141">
-        <v>13.7</v>
+        <v>13.75</v>
       </c>
       <c r="G141">
-        <v>-0.3</v>
+        <v>-0.25</v>
       </c>
       <c r="H141">
-        <v>376302.1</v>
+        <v>383645.5</v>
       </c>
       <c r="I141" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Generated results using v30.1 on 120723
</commit_message>
<xml_diff>
--- a/results/multi_city/AP/desc_stats.xlsx
+++ b/results/multi_city/AP/desc_stats.xlsx
@@ -1558,7 +1558,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>12.69</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -1940,88 +1940,88 @@
         </is>
       </c>
       <c r="B3">
-        <v>48414.1</v>
+        <v>45879.9</v>
       </c>
       <c r="C3">
-        <v>44487.2</v>
+        <v>42483.8</v>
       </c>
       <c r="D3">
-        <v>587390.8</v>
+        <v>567870.8</v>
       </c>
       <c r="E3">
-        <v>1550837</v>
+        <v>1440897</v>
       </c>
       <c r="F3">
-        <v>2964297.1</v>
+        <v>2536340.4</v>
       </c>
       <c r="G3">
-        <v>499054.8</v>
+        <v>476354.2</v>
       </c>
       <c r="H3">
-        <v>5126.4</v>
+        <v>4980.1</v>
       </c>
       <c r="I3">
-        <v>31542.1</v>
+        <v>29753.9</v>
       </c>
       <c r="J3">
-        <v>1142859</v>
+        <v>1087094.8</v>
       </c>
       <c r="K3">
-        <v>48335.4</v>
+        <v>46113</v>
       </c>
       <c r="L3">
-        <v>487784.7</v>
+        <v>465384.6</v>
       </c>
       <c r="M3">
-        <v>3264287.9</v>
+        <v>2962408.3</v>
       </c>
       <c r="N3">
-        <v>293964.3</v>
+        <v>258540.1</v>
       </c>
       <c r="O3">
-        <v>26651.9</v>
+        <v>26140.6</v>
       </c>
       <c r="P3">
-        <v>79985.60000000001</v>
+        <v>77692.89999999999</v>
       </c>
       <c r="Q3">
-        <v>59397</v>
+        <v>57215.1</v>
       </c>
       <c r="R3">
-        <v>417495.2</v>
+        <v>396584.2</v>
       </c>
       <c r="S3">
-        <v>2722312.2</v>
+        <v>2593675.4</v>
       </c>
       <c r="T3">
-        <v>8888</v>
+        <v>8725</v>
       </c>
       <c r="U3">
-        <v>8574.1</v>
+        <v>8505.5</v>
       </c>
       <c r="V3">
-        <v>388200.1</v>
+        <v>338016.6</v>
       </c>
       <c r="W3">
-        <v>2117441.3</v>
+        <v>2116302.5</v>
       </c>
       <c r="X3">
-        <v>1748485.7</v>
+        <v>1736315</v>
       </c>
       <c r="Y3">
-        <v>3885930.4</v>
+        <v>3899250</v>
       </c>
       <c r="Z3">
-        <v>217618.6</v>
+        <v>208515.3</v>
       </c>
       <c r="AA3">
-        <v>6834.4</v>
+        <v>6297.4</v>
       </c>
       <c r="AB3">
-        <v>494683.9</v>
+        <v>443933.3</v>
       </c>
       <c r="AC3">
-        <v>403289.8</v>
+        <v>363315.7</v>
       </c>
     </row>
     <row r="4">
@@ -2031,88 +2031,88 @@
         </is>
       </c>
       <c r="B4">
-        <v>51977.2</v>
+        <v>52149.7</v>
       </c>
       <c r="C4">
-        <v>50418.8</v>
+        <v>50547.4</v>
       </c>
       <c r="D4">
-        <v>620064.1</v>
+        <v>621957</v>
       </c>
       <c r="E4">
-        <v>1756205.4</v>
+        <v>1748564.4</v>
       </c>
       <c r="F4">
-        <v>3606770.2</v>
+        <v>3553882</v>
       </c>
       <c r="G4">
-        <v>578540.6</v>
+        <v>568810.1</v>
       </c>
       <c r="H4">
-        <v>5449.8</v>
+        <v>5466.1</v>
       </c>
       <c r="I4">
-        <v>35065.2</v>
+        <v>35214.6</v>
       </c>
       <c r="J4">
-        <v>1222888.1</v>
+        <v>1222968.6</v>
       </c>
       <c r="K4">
-        <v>51895.2</v>
+        <v>52052.6</v>
       </c>
       <c r="L4">
-        <v>610751.9</v>
+        <v>604134.8</v>
       </c>
       <c r="M4">
-        <v>3707770.6</v>
+        <v>3702855.4</v>
       </c>
       <c r="N4">
-        <v>341094.4</v>
+        <v>340990</v>
       </c>
       <c r="O4">
-        <v>28101.3</v>
+        <v>28106.3</v>
       </c>
       <c r="P4">
-        <v>87167.10000000001</v>
+        <v>86756.7</v>
       </c>
       <c r="Q4">
-        <v>63834.8</v>
+        <v>64052.2</v>
       </c>
       <c r="R4">
-        <v>456489.4</v>
+        <v>456895.7</v>
       </c>
       <c r="S4">
-        <v>2957194.8</v>
+        <v>2969372.6</v>
       </c>
       <c r="T4">
-        <v>9232.1</v>
+        <v>9227.700000000001</v>
       </c>
       <c r="U4">
-        <v>8865.6</v>
+        <v>8894.200000000001</v>
       </c>
       <c r="V4">
-        <v>487932.1</v>
+        <v>484473.9</v>
       </c>
       <c r="W4">
-        <v>2694343.8</v>
+        <v>2632264.5</v>
       </c>
       <c r="X4">
-        <v>1818676.7</v>
+        <v>1810657.2</v>
       </c>
       <c r="Y4">
-        <v>4040523.4</v>
+        <v>4042695.7</v>
       </c>
       <c r="Z4">
-        <v>335537.3</v>
+        <v>329844.7</v>
       </c>
       <c r="AA4">
-        <v>9399.700000000001</v>
+        <v>9152.799999999999</v>
       </c>
       <c r="AB4">
-        <v>570903.9</v>
+        <v>564421.1</v>
       </c>
       <c r="AC4">
-        <v>500335.8</v>
+        <v>497761.3</v>
       </c>
     </row>
     <row r="5">
@@ -2122,88 +2122,88 @@
         </is>
       </c>
       <c r="B5">
-        <v>46124.8</v>
+        <v>48423.9</v>
       </c>
       <c r="C5">
-        <v>42308.8</v>
+        <v>44501.8</v>
       </c>
       <c r="D5">
-        <v>563626.8</v>
+        <v>587430</v>
       </c>
       <c r="E5">
-        <v>1433623.7</v>
+        <v>1554472.6</v>
       </c>
       <c r="F5">
-        <v>2533020.5</v>
+        <v>2974962.5</v>
       </c>
       <c r="G5">
-        <v>478203.9</v>
+        <v>498324.2</v>
       </c>
       <c r="H5">
-        <v>4980.2</v>
+        <v>5121.5</v>
       </c>
       <c r="I5">
-        <v>29255.8</v>
+        <v>31584.8</v>
       </c>
       <c r="J5">
-        <v>1084843.3</v>
+        <v>1142636.6</v>
       </c>
       <c r="K5">
-        <v>46635.5</v>
+        <v>48366</v>
       </c>
       <c r="L5">
-        <v>464144.9</v>
+        <v>489237.4</v>
       </c>
       <c r="M5">
-        <v>2968397.2</v>
+        <v>3263944.7</v>
       </c>
       <c r="N5">
-        <v>262014.5</v>
+        <v>291440</v>
       </c>
       <c r="O5">
-        <v>26164.4</v>
+        <v>26650.9</v>
       </c>
       <c r="P5">
-        <v>76880</v>
+        <v>80342</v>
       </c>
       <c r="Q5">
-        <v>57355.5</v>
+        <v>59442.1</v>
       </c>
       <c r="R5">
-        <v>396086.4</v>
+        <v>417721.6</v>
       </c>
       <c r="S5">
-        <v>2542699.8</v>
+        <v>2726886.6</v>
       </c>
       <c r="T5">
-        <v>8677.299999999999</v>
+        <v>8891.299999999999</v>
       </c>
       <c r="U5">
-        <v>8431</v>
+        <v>8585.799999999999</v>
       </c>
       <c r="V5">
-        <v>343146.4</v>
+        <v>388626.7</v>
       </c>
       <c r="W5">
-        <v>2119750.7</v>
+        <v>2114583.8</v>
       </c>
       <c r="X5">
-        <v>1736083.1</v>
+        <v>1742573.5</v>
       </c>
       <c r="Y5">
-        <v>3909321.5</v>
+        <v>3884479.9</v>
       </c>
       <c r="Z5">
-        <v>206331.1</v>
+        <v>217606.3</v>
       </c>
       <c r="AA5">
-        <v>6445.5</v>
+        <v>6825.6</v>
       </c>
       <c r="AB5">
-        <v>445449</v>
+        <v>493921.8</v>
       </c>
       <c r="AC5">
-        <v>375481</v>
+        <v>398600.3</v>
       </c>
     </row>
     <row r="6">
@@ -2213,88 +2213,88 @@
         </is>
       </c>
       <c r="B6">
-        <v>60203.8</v>
+        <v>60868.5</v>
       </c>
       <c r="C6">
-        <v>56929</v>
+        <v>58233.9</v>
       </c>
       <c r="D6">
-        <v>648651.4</v>
+        <v>649705.1</v>
       </c>
       <c r="E6">
-        <v>1513636.8</v>
+        <v>1514132.7</v>
       </c>
       <c r="F6">
-        <v>2941384</v>
+        <v>2926970.9</v>
       </c>
       <c r="G6">
-        <v>480003</v>
+        <v>482437.3</v>
       </c>
       <c r="H6">
-        <v>6131.2</v>
+        <v>6223.4</v>
       </c>
       <c r="I6">
-        <v>45077.8</v>
+        <v>45911.6</v>
       </c>
       <c r="J6">
-        <v>1406225.4</v>
+        <v>1409157.2</v>
       </c>
       <c r="K6">
-        <v>60683.8</v>
+        <v>60782.5</v>
       </c>
       <c r="L6">
-        <v>476418.3</v>
+        <v>475088.1</v>
       </c>
       <c r="M6">
-        <v>3292816</v>
+        <v>3287025</v>
       </c>
       <c r="N6">
-        <v>284404.7</v>
+        <v>287970.5</v>
       </c>
       <c r="O6">
-        <v>30612</v>
+        <v>30745.5</v>
       </c>
       <c r="P6">
-        <v>141011.4</v>
+        <v>140491.6</v>
       </c>
       <c r="Q6">
-        <v>69908</v>
+        <v>69724.8</v>
       </c>
       <c r="R6">
-        <v>449972</v>
+        <v>450824.8</v>
       </c>
       <c r="S6">
-        <v>3500739.2</v>
+        <v>3504749.4</v>
       </c>
       <c r="T6">
-        <v>9850.299999999999</v>
+        <v>9930.299999999999</v>
       </c>
       <c r="U6">
-        <v>9456.5</v>
+        <v>9491.6</v>
       </c>
       <c r="V6">
-        <v>384853.7</v>
+        <v>382943</v>
       </c>
       <c r="W6">
-        <v>2084559.9</v>
+        <v>2085942.9</v>
       </c>
       <c r="X6">
-        <v>1764447.9</v>
+        <v>1759289.8</v>
       </c>
       <c r="Y6">
-        <v>4119062.6</v>
+        <v>4126374.9</v>
       </c>
       <c r="Z6">
-        <v>232812</v>
+        <v>228891.4</v>
       </c>
       <c r="AA6">
-        <v>6259</v>
+        <v>6493.2</v>
       </c>
       <c r="AB6">
-        <v>480470.6</v>
+        <v>481812.4</v>
       </c>
       <c r="AC6">
-        <v>383645.5</v>
+        <v>371165.8</v>
       </c>
     </row>
   </sheetData>
@@ -2397,16 +2397,16 @@
         </is>
       </c>
       <c r="B3">
-        <v>11.2</v>
+        <v>10.9</v>
       </c>
       <c r="C3">
         <v>10.4</v>
       </c>
       <c r="D3">
-        <v>11</v>
+        <v>10.8</v>
       </c>
       <c r="E3">
-        <v>12</v>
+        <v>11.5</v>
       </c>
       <c r="F3">
         <v>10.39</v>
@@ -2415,7 +2415,7 @@
         <v>-0.1</v>
       </c>
       <c r="H3">
-        <v>48414.1</v>
+        <v>45879.9</v>
       </c>
       <c r="I3" t="inlineStr">
         <is>
@@ -2442,13 +2442,13 @@
         <v>12.1</v>
       </c>
       <c r="F4">
-        <v>10.68</v>
+        <v>10.69</v>
       </c>
       <c r="G4">
-        <v>0.19</v>
+        <v>0.2</v>
       </c>
       <c r="H4">
-        <v>51977.2</v>
+        <v>52149.7</v>
       </c>
       <c r="I4" t="inlineStr">
         <is>
@@ -2463,25 +2463,25 @@
         </is>
       </c>
       <c r="B5">
-        <v>10.9</v>
+        <v>11.1</v>
       </c>
       <c r="C5">
         <v>10.2</v>
       </c>
       <c r="D5">
-        <v>10.8</v>
+        <v>11</v>
       </c>
       <c r="E5">
-        <v>11.6</v>
+        <v>12</v>
       </c>
       <c r="F5">
-        <v>10.23</v>
+        <v>10.2</v>
       </c>
       <c r="G5">
-        <v>-0.26</v>
+        <v>-0.29</v>
       </c>
       <c r="H5">
-        <v>46124.8</v>
+        <v>48423.9</v>
       </c>
       <c r="I5" t="inlineStr">
         <is>
@@ -2508,13 +2508,13 @@
         <v>11.8</v>
       </c>
       <c r="F6">
-        <v>10.41</v>
+        <v>10.43</v>
       </c>
       <c r="G6">
-        <v>-0.08</v>
+        <v>-0.06</v>
       </c>
       <c r="H6">
-        <v>60203.8</v>
+        <v>60868.5</v>
       </c>
       <c r="I6" t="inlineStr">
         <is>
@@ -2562,16 +2562,16 @@
         </is>
       </c>
       <c r="B8">
-        <v>13.3</v>
+        <v>13</v>
       </c>
       <c r="C8">
         <v>12.4</v>
       </c>
       <c r="D8">
-        <v>13.1</v>
+        <v>12.9</v>
       </c>
       <c r="E8">
-        <v>14.4</v>
+        <v>13.8</v>
       </c>
       <c r="F8">
         <v>12.36</v>
@@ -2580,7 +2580,7 @@
         <v>-0.2</v>
       </c>
       <c r="H8">
-        <v>44487.2</v>
+        <v>42483.8</v>
       </c>
       <c r="I8" t="inlineStr">
         <is>
@@ -2613,7 +2613,7 @@
         <v>0.41</v>
       </c>
       <c r="H9">
-        <v>50418.8</v>
+        <v>50547.4</v>
       </c>
       <c r="I9" t="inlineStr">
         <is>
@@ -2628,25 +2628,25 @@
         </is>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>13.3</v>
       </c>
       <c r="C10">
         <v>12.2</v>
       </c>
       <c r="D10">
-        <v>12.9</v>
+        <v>13.1</v>
       </c>
       <c r="E10">
-        <v>13.8</v>
+        <v>14.4</v>
       </c>
       <c r="F10">
-        <v>12.19</v>
+        <v>12.21</v>
       </c>
       <c r="G10">
-        <v>-0.37</v>
+        <v>-0.35</v>
       </c>
       <c r="H10">
-        <v>42308.8</v>
+        <v>44501.8</v>
       </c>
       <c r="I10" t="inlineStr">
         <is>
@@ -2676,10 +2676,10 @@
         <v>12.4</v>
       </c>
       <c r="G11">
-        <v>-0.17</v>
+        <v>-0.16</v>
       </c>
       <c r="H11">
-        <v>56929</v>
+        <v>58233.9</v>
       </c>
       <c r="I11" t="inlineStr">
         <is>
@@ -2727,16 +2727,16 @@
         </is>
       </c>
       <c r="B13">
-        <v>17.9</v>
+        <v>17.7</v>
       </c>
       <c r="C13">
         <v>16.9</v>
       </c>
       <c r="D13">
-        <v>17.5</v>
+        <v>17.3</v>
       </c>
       <c r="E13">
-        <v>19.6</v>
+        <v>19.2</v>
       </c>
       <c r="F13">
         <v>16.92</v>
@@ -2745,7 +2745,7 @@
         <v>-0.08</v>
       </c>
       <c r="H13">
-        <v>587390.8</v>
+        <v>567870.8</v>
       </c>
       <c r="I13" t="inlineStr">
         <is>
@@ -2772,13 +2772,13 @@
         <v>19.8</v>
       </c>
       <c r="F14">
-        <v>17.29</v>
+        <v>17.28</v>
       </c>
       <c r="G14">
-        <v>0.29</v>
+        <v>0.28</v>
       </c>
       <c r="H14">
-        <v>620064.1</v>
+        <v>621957</v>
       </c>
       <c r="I14" t="inlineStr">
         <is>
@@ -2793,16 +2793,16 @@
         </is>
       </c>
       <c r="B15">
-        <v>17.6</v>
+        <v>17.8</v>
       </c>
       <c r="C15">
         <v>16.7</v>
       </c>
       <c r="D15">
-        <v>17.3</v>
+        <v>17.5</v>
       </c>
       <c r="E15">
-        <v>19.2</v>
+        <v>19.6</v>
       </c>
       <c r="F15">
         <v>16.74</v>
@@ -2811,7 +2811,7 @@
         <v>-0.26</v>
       </c>
       <c r="H15">
-        <v>563626.8</v>
+        <v>587430</v>
       </c>
       <c r="I15" t="inlineStr">
         <is>
@@ -2844,7 +2844,7 @@
         <v>-0.08</v>
       </c>
       <c r="H16">
-        <v>648651.4</v>
+        <v>649705.1</v>
       </c>
       <c r="I16" t="inlineStr">
         <is>
@@ -2859,19 +2859,19 @@
         </is>
       </c>
       <c r="B17">
-        <v>26.8</v>
+        <v>14.2</v>
       </c>
       <c r="C17">
-        <v>24</v>
+        <v>12.7</v>
       </c>
       <c r="D17">
-        <v>26.3</v>
+        <v>13.9</v>
       </c>
       <c r="E17">
-        <v>29.9</v>
+        <v>15.8</v>
       </c>
       <c r="F17">
-        <v>24</v>
+        <v>12.69</v>
       </c>
       <c r="G17">
         <v>0</v>
@@ -2892,25 +2892,25 @@
         </is>
       </c>
       <c r="B18">
-        <v>26.8</v>
+        <v>14.2</v>
       </c>
       <c r="C18">
-        <v>23.8</v>
+        <v>12.6</v>
       </c>
       <c r="D18">
-        <v>26.3</v>
+        <v>13.9</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>15.7</v>
       </c>
       <c r="F18">
-        <v>23.85</v>
+        <v>12.61</v>
       </c>
       <c r="G18">
-        <v>-0.15</v>
+        <v>-0.08</v>
       </c>
       <c r="H18">
-        <v>1550837</v>
+        <v>1440897</v>
       </c>
       <c r="I18" t="inlineStr">
         <is>
@@ -2925,25 +2925,25 @@
         </is>
       </c>
       <c r="B19">
-        <v>26.7</v>
+        <v>14.1</v>
       </c>
       <c r="C19">
-        <v>24</v>
+        <v>12.7</v>
       </c>
       <c r="D19">
-        <v>26.2</v>
+        <v>13.9</v>
       </c>
       <c r="E19">
-        <v>29.7</v>
+        <v>15.7</v>
       </c>
       <c r="F19">
-        <v>23.96</v>
+        <v>12.67</v>
       </c>
       <c r="G19">
-        <v>-0.04</v>
+        <v>-0.02</v>
       </c>
       <c r="H19">
-        <v>1756205.4</v>
+        <v>1748564.4</v>
       </c>
       <c r="I19" t="inlineStr">
         <is>
@@ -2958,25 +2958,25 @@
         </is>
       </c>
       <c r="B20">
-        <v>26.8</v>
+        <v>14.2</v>
       </c>
       <c r="C20">
-        <v>24</v>
+        <v>12.7</v>
       </c>
       <c r="D20">
-        <v>26.4</v>
+        <v>13.9</v>
       </c>
       <c r="E20">
-        <v>29.8</v>
+        <v>15.9</v>
       </c>
       <c r="F20">
-        <v>24.01</v>
+        <v>12.68</v>
       </c>
       <c r="G20">
-        <v>0.01</v>
+        <v>-0.01</v>
       </c>
       <c r="H20">
-        <v>1433623.7</v>
+        <v>1554472.6</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
@@ -2991,25 +2991,25 @@
         </is>
       </c>
       <c r="B21">
-        <v>26.5</v>
+        <v>14</v>
       </c>
       <c r="C21">
-        <v>23.8</v>
+        <v>12.6</v>
       </c>
       <c r="D21">
-        <v>26</v>
+        <v>13.8</v>
       </c>
       <c r="E21">
-        <v>29.4</v>
+        <v>15.5</v>
       </c>
       <c r="F21">
-        <v>23.78</v>
+        <v>12.57</v>
       </c>
       <c r="G21">
-        <v>-0.22</v>
+        <v>-0.12</v>
       </c>
       <c r="H21">
-        <v>1513636.8</v>
+        <v>1514132.7</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
@@ -3057,16 +3057,16 @@
         </is>
       </c>
       <c r="B23">
-        <v>14.6</v>
+        <v>14.5</v>
       </c>
       <c r="C23">
         <v>13.9</v>
       </c>
       <c r="D23">
-        <v>14.4</v>
+        <v>14.3</v>
       </c>
       <c r="E23">
-        <v>15.7</v>
+        <v>15.5</v>
       </c>
       <c r="F23">
         <v>13.89</v>
@@ -3075,7 +3075,7 @@
         <v>-0.11</v>
       </c>
       <c r="H23">
-        <v>2964297.1</v>
+        <v>2536340.4</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -3102,13 +3102,13 @@
         <v>15.9</v>
       </c>
       <c r="F24">
-        <v>14.12</v>
+        <v>14.1</v>
       </c>
       <c r="G24">
-        <v>0.12</v>
+        <v>0.1</v>
       </c>
       <c r="H24">
-        <v>3606770.2</v>
+        <v>3553882</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -3123,25 +3123,25 @@
         </is>
       </c>
       <c r="B25">
-        <v>14.5</v>
+        <v>14.6</v>
       </c>
       <c r="C25">
         <v>13.8</v>
       </c>
       <c r="D25">
-        <v>14.3</v>
+        <v>14.4</v>
       </c>
       <c r="E25">
-        <v>15.5</v>
+        <v>15.7</v>
       </c>
       <c r="F25">
-        <v>13.82</v>
+        <v>13.81</v>
       </c>
       <c r="G25">
-        <v>-0.18</v>
+        <v>-0.19</v>
       </c>
       <c r="H25">
-        <v>2533020.5</v>
+        <v>2974962.5</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
@@ -3174,7 +3174,7 @@
         <v>-0.15</v>
       </c>
       <c r="H26">
-        <v>2941384</v>
+        <v>2926970.9</v>
       </c>
       <c r="I26" t="inlineStr">
         <is>
@@ -3222,25 +3222,25 @@
         </is>
       </c>
       <c r="B28">
-        <v>25.8</v>
+        <v>25.9</v>
       </c>
       <c r="C28">
         <v>23.9</v>
       </c>
       <c r="D28">
-        <v>25</v>
+        <v>25.2</v>
       </c>
       <c r="E28">
-        <v>28.3</v>
+        <v>28.2</v>
       </c>
       <c r="F28">
-        <v>23.9</v>
+        <v>23.89</v>
       </c>
       <c r="G28">
-        <v>-0.15</v>
+        <v>-0.16</v>
       </c>
       <c r="H28">
-        <v>499054.8</v>
+        <v>476354.2</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -3255,7 +3255,7 @@
         </is>
       </c>
       <c r="B29">
-        <v>25.9</v>
+        <v>25.8</v>
       </c>
       <c r="C29">
         <v>24</v>
@@ -3267,13 +3267,13 @@
         <v>28.1</v>
       </c>
       <c r="F29">
-        <v>24.04</v>
+        <v>24.02</v>
       </c>
       <c r="G29">
-        <v>-0.01</v>
+        <v>-0.03</v>
       </c>
       <c r="H29">
-        <v>578540.6</v>
+        <v>568810.1</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -3288,25 +3288,25 @@
         </is>
       </c>
       <c r="B30">
-        <v>26</v>
+        <v>25.9</v>
       </c>
       <c r="C30">
-        <v>24.2</v>
+        <v>24.1</v>
       </c>
       <c r="D30">
-        <v>25.2</v>
+        <v>25</v>
       </c>
       <c r="E30">
         <v>28.3</v>
       </c>
       <c r="F30">
-        <v>24.18</v>
+        <v>24.11</v>
       </c>
       <c r="G30">
-        <v>0.13</v>
+        <v>0.06</v>
       </c>
       <c r="H30">
-        <v>478203.9</v>
+        <v>498324.2</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
@@ -3333,13 +3333,13 @@
         <v>27.7</v>
       </c>
       <c r="F31">
-        <v>23.79</v>
+        <v>23.8</v>
       </c>
       <c r="G31">
-        <v>-0.26</v>
+        <v>-0.25</v>
       </c>
       <c r="H31">
-        <v>480003</v>
+        <v>482437.3</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
@@ -3387,25 +3387,25 @@
         </is>
       </c>
       <c r="B33">
-        <v>16.7</v>
+        <v>16.4</v>
       </c>
       <c r="C33">
         <v>15.4</v>
       </c>
       <c r="D33">
-        <v>16.4</v>
+        <v>16.2</v>
       </c>
       <c r="E33">
-        <v>18.1</v>
+        <v>17.5</v>
       </c>
       <c r="F33">
-        <v>15.44</v>
+        <v>15.43</v>
       </c>
       <c r="G33">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H33">
-        <v>5126.4</v>
+        <v>4980.1</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -3429,7 +3429,7 @@
         <v>16.8</v>
       </c>
       <c r="E34">
-        <v>18</v>
+        <v>18.1</v>
       </c>
       <c r="F34">
         <v>15.82</v>
@@ -3438,7 +3438,7 @@
         <v>0.22</v>
       </c>
       <c r="H34">
-        <v>5449.8</v>
+        <v>5466.1</v>
       </c>
       <c r="I34" t="inlineStr">
         <is>
@@ -3453,16 +3453,16 @@
         </is>
       </c>
       <c r="B35">
-        <v>16.4</v>
+        <v>16.7</v>
       </c>
       <c r="C35">
         <v>15.4</v>
       </c>
       <c r="D35">
-        <v>16.3</v>
+        <v>16.4</v>
       </c>
       <c r="E35">
-        <v>17.5</v>
+        <v>18.1</v>
       </c>
       <c r="F35">
         <v>15.36</v>
@@ -3471,7 +3471,7 @@
         <v>-0.24</v>
       </c>
       <c r="H35">
-        <v>4980.2</v>
+        <v>5121.5</v>
       </c>
       <c r="I35" t="inlineStr">
         <is>
@@ -3501,10 +3501,10 @@
         <v>15.44</v>
       </c>
       <c r="G36">
-        <v>-0.16</v>
+        <v>-0.17</v>
       </c>
       <c r="H36">
-        <v>6131.2</v>
+        <v>6223.4</v>
       </c>
       <c r="I36" t="inlineStr">
         <is>
@@ -3552,25 +3552,25 @@
         </is>
       </c>
       <c r="B38">
-        <v>14.9</v>
+        <v>14.5</v>
       </c>
       <c r="C38">
         <v>13.7</v>
       </c>
       <c r="D38">
-        <v>14.6</v>
+        <v>14.3</v>
       </c>
       <c r="E38">
-        <v>15.9</v>
+        <v>15.4</v>
       </c>
       <c r="F38">
         <v>13.73</v>
       </c>
       <c r="G38">
-        <v>-0.16</v>
+        <v>-0.15</v>
       </c>
       <c r="H38">
-        <v>31542.1</v>
+        <v>29753.9</v>
       </c>
       <c r="I38" t="inlineStr">
         <is>
@@ -3591,7 +3591,7 @@
         <v>14.3</v>
       </c>
       <c r="D39">
-        <v>15.1</v>
+        <v>15.2</v>
       </c>
       <c r="E39">
         <v>16.4</v>
@@ -3603,7 +3603,7 @@
         <v>0.42</v>
       </c>
       <c r="H39">
-        <v>35065.2</v>
+        <v>35214.6</v>
       </c>
       <c r="I39" t="inlineStr">
         <is>
@@ -3618,25 +3618,25 @@
         </is>
       </c>
       <c r="B40">
-        <v>14.4</v>
+        <v>14.8</v>
       </c>
       <c r="C40">
-        <v>13.4</v>
+        <v>13.5</v>
       </c>
       <c r="D40">
-        <v>14.2</v>
+        <v>14.6</v>
       </c>
       <c r="E40">
-        <v>15.3</v>
+        <v>15.9</v>
       </c>
       <c r="F40">
-        <v>13.4</v>
+        <v>13.47</v>
       </c>
       <c r="G40">
-        <v>-0.48</v>
+        <v>-0.41</v>
       </c>
       <c r="H40">
-        <v>29255.8</v>
+        <v>31584.8</v>
       </c>
       <c r="I40" t="inlineStr">
         <is>
@@ -3663,13 +3663,13 @@
         <v>15.7</v>
       </c>
       <c r="F41">
-        <v>13.78</v>
+        <v>13.8</v>
       </c>
       <c r="G41">
-        <v>-0.11</v>
+        <v>-0.08</v>
       </c>
       <c r="H41">
-        <v>45077.8</v>
+        <v>45911.6</v>
       </c>
       <c r="I41" t="inlineStr">
         <is>
@@ -3717,25 +3717,25 @@
         </is>
       </c>
       <c r="B43">
-        <v>16.1</v>
+        <v>15.9</v>
       </c>
       <c r="C43">
         <v>14.9</v>
       </c>
       <c r="D43">
-        <v>16</v>
+        <v>15.7</v>
       </c>
       <c r="E43">
-        <v>17.4</v>
+        <v>17</v>
       </c>
       <c r="F43">
         <v>14.95</v>
       </c>
       <c r="G43">
-        <v>-0.14</v>
+        <v>-0.15</v>
       </c>
       <c r="H43">
-        <v>1142859</v>
+        <v>1087094.8</v>
       </c>
       <c r="I43" t="inlineStr">
         <is>
@@ -3756,19 +3756,19 @@
         <v>15.4</v>
       </c>
       <c r="D44">
-        <v>16.4</v>
+        <v>16.3</v>
       </c>
       <c r="E44">
         <v>17.7</v>
       </c>
       <c r="F44">
-        <v>15.37</v>
+        <v>15.36</v>
       </c>
       <c r="G44">
-        <v>0.28</v>
+        <v>0.27</v>
       </c>
       <c r="H44">
-        <v>1222888.1</v>
+        <v>1222968.6</v>
       </c>
       <c r="I44" t="inlineStr">
         <is>
@@ -3783,16 +3783,16 @@
         </is>
       </c>
       <c r="B45">
-        <v>15.8</v>
+        <v>16.1</v>
       </c>
       <c r="C45">
         <v>14.7</v>
       </c>
       <c r="D45">
-        <v>15.7</v>
+        <v>16</v>
       </c>
       <c r="E45">
-        <v>17</v>
+        <v>17.4</v>
       </c>
       <c r="F45">
         <v>14.74</v>
@@ -3801,7 +3801,7 @@
         <v>-0.35</v>
       </c>
       <c r="H45">
-        <v>1084843.3</v>
+        <v>1142636.6</v>
       </c>
       <c r="I45" t="inlineStr">
         <is>
@@ -3828,13 +3828,13 @@
         <v>17.1</v>
       </c>
       <c r="F46">
-        <v>14.99</v>
+        <v>15</v>
       </c>
       <c r="G46">
-        <v>-0.1</v>
+        <v>-0.09</v>
       </c>
       <c r="H46">
-        <v>1406225.4</v>
+        <v>1409157.2</v>
       </c>
       <c r="I46" t="inlineStr">
         <is>
@@ -3882,16 +3882,16 @@
         </is>
       </c>
       <c r="B48">
-        <v>12.4</v>
+        <v>12.1</v>
       </c>
       <c r="C48">
         <v>11.6</v>
       </c>
       <c r="D48">
-        <v>12.2</v>
+        <v>12</v>
       </c>
       <c r="E48">
-        <v>13.3</v>
+        <v>12.9</v>
       </c>
       <c r="F48">
         <v>11.56</v>
@@ -3900,7 +3900,7 @@
         <v>-0.12</v>
       </c>
       <c r="H48">
-        <v>48335.4</v>
+        <v>46113</v>
       </c>
       <c r="I48" t="inlineStr">
         <is>
@@ -3933,7 +3933,7 @@
         <v>0.2</v>
       </c>
       <c r="H49">
-        <v>51895.2</v>
+        <v>52052.6</v>
       </c>
       <c r="I49" t="inlineStr">
         <is>
@@ -3948,25 +3948,25 @@
         </is>
       </c>
       <c r="B50">
+        <v>12.3</v>
+      </c>
+      <c r="C50">
+        <v>11.4</v>
+      </c>
+      <c r="D50">
         <v>12.2</v>
       </c>
-      <c r="C50">
-        <v>11.5</v>
-      </c>
-      <c r="D50">
-        <v>12</v>
-      </c>
       <c r="E50">
-        <v>12.9</v>
+        <v>13.3</v>
       </c>
       <c r="F50">
-        <v>11.46</v>
+        <v>11.41</v>
       </c>
       <c r="G50">
-        <v>-0.23</v>
+        <v>-0.27</v>
       </c>
       <c r="H50">
-        <v>46635.5</v>
+        <v>48366</v>
       </c>
       <c r="I50" t="inlineStr">
         <is>
@@ -3990,16 +3990,16 @@
         <v>12.2</v>
       </c>
       <c r="E51">
-        <v>13</v>
+        <v>13.1</v>
       </c>
       <c r="F51">
-        <v>11.57</v>
+        <v>11.6</v>
       </c>
       <c r="G51">
-        <v>-0.11</v>
+        <v>-0.08</v>
       </c>
       <c r="H51">
-        <v>60683.8</v>
+        <v>60782.5</v>
       </c>
       <c r="I51" t="inlineStr">
         <is>
@@ -4047,16 +4047,16 @@
         </is>
       </c>
       <c r="B53">
-        <v>22.4</v>
+        <v>22.5</v>
       </c>
       <c r="C53">
-        <v>20.9</v>
+        <v>21</v>
       </c>
       <c r="D53">
-        <v>22.3</v>
+        <v>22.5</v>
       </c>
       <c r="E53">
-        <v>24</v>
+        <v>24.1</v>
       </c>
       <c r="F53">
         <v>20.95</v>
@@ -4065,7 +4065,7 @@
         <v>-0.14</v>
       </c>
       <c r="H53">
-        <v>487784.7</v>
+        <v>465384.6</v>
       </c>
       <c r="I53" t="inlineStr">
         <is>
@@ -4092,13 +4092,13 @@
         <v>24.1</v>
       </c>
       <c r="F54">
-        <v>21.13</v>
+        <v>21.12</v>
       </c>
       <c r="G54">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="H54">
-        <v>610751.9</v>
+        <v>604134.8</v>
       </c>
       <c r="I54" t="inlineStr">
         <is>
@@ -4113,25 +4113,25 @@
         </is>
       </c>
       <c r="B55">
-        <v>22.6</v>
+        <v>22.5</v>
       </c>
       <c r="C55">
         <v>21.2</v>
       </c>
       <c r="D55">
-        <v>22.5</v>
+        <v>22.3</v>
       </c>
       <c r="E55">
-        <v>24.1</v>
+        <v>24</v>
       </c>
       <c r="F55">
-        <v>21.21</v>
+        <v>21.2</v>
       </c>
       <c r="G55">
-        <v>0.12</v>
+        <v>0.11</v>
       </c>
       <c r="H55">
-        <v>464144.9</v>
+        <v>489237.4</v>
       </c>
       <c r="I55" t="inlineStr">
         <is>
@@ -4155,7 +4155,7 @@
         <v>22</v>
       </c>
       <c r="E56">
-        <v>23.6</v>
+        <v>23.7</v>
       </c>
       <c r="F56">
         <v>20.89</v>
@@ -4164,7 +4164,7 @@
         <v>-0.2</v>
       </c>
       <c r="H56">
-        <v>476418.3</v>
+        <v>475088.1</v>
       </c>
       <c r="I56" t="inlineStr">
         <is>
@@ -4212,16 +4212,16 @@
         </is>
       </c>
       <c r="B58">
-        <v>54.6</v>
+        <v>53.1</v>
       </c>
       <c r="C58">
         <v>49.8</v>
       </c>
       <c r="D58">
-        <v>53.9</v>
+        <v>52.5</v>
       </c>
       <c r="E58">
-        <v>59.1</v>
+        <v>57.3</v>
       </c>
       <c r="F58">
         <v>49.79</v>
@@ -4230,7 +4230,7 @@
         <v>-0.21</v>
       </c>
       <c r="H58">
-        <v>3264287.9</v>
+        <v>2962408.3</v>
       </c>
       <c r="I58" t="inlineStr">
         <is>
@@ -4257,13 +4257,13 @@
         <v>60.4</v>
       </c>
       <c r="F59">
-        <v>51.24</v>
+        <v>51.23</v>
       </c>
       <c r="G59">
-        <v>1.24</v>
+        <v>1.23</v>
       </c>
       <c r="H59">
-        <v>3707770.6</v>
+        <v>3702855.4</v>
       </c>
       <c r="I59" t="inlineStr">
         <is>
@@ -4278,25 +4278,25 @@
         </is>
       </c>
       <c r="B60">
-        <v>53.1</v>
+        <v>54.5</v>
       </c>
       <c r="C60">
         <v>48.7</v>
       </c>
       <c r="D60">
-        <v>52.5</v>
+        <v>53.9</v>
       </c>
       <c r="E60">
-        <v>57.3</v>
+        <v>59.1</v>
       </c>
       <c r="F60">
-        <v>48.73</v>
+        <v>48.72</v>
       </c>
       <c r="G60">
-        <v>-1.27</v>
+        <v>-1.28</v>
       </c>
       <c r="H60">
-        <v>2968397.2</v>
+        <v>3263944.7</v>
       </c>
       <c r="I60" t="inlineStr">
         <is>
@@ -4323,13 +4323,13 @@
         <v>59</v>
       </c>
       <c r="F61">
-        <v>50.33</v>
+        <v>50.31</v>
       </c>
       <c r="G61">
-        <v>0.33</v>
+        <v>0.31</v>
       </c>
       <c r="H61">
-        <v>3292816</v>
+        <v>3287025</v>
       </c>
       <c r="I61" t="inlineStr">
         <is>
@@ -4377,25 +4377,25 @@
         </is>
       </c>
       <c r="B63">
-        <v>16.7</v>
+        <v>16.6</v>
       </c>
       <c r="C63">
         <v>15.5</v>
       </c>
       <c r="D63">
-        <v>16.5</v>
+        <v>16.6</v>
       </c>
       <c r="E63">
-        <v>18</v>
+        <v>17.9</v>
       </c>
       <c r="F63">
         <v>15.47</v>
       </c>
       <c r="G63">
-        <v>-0.1</v>
+        <v>-0.11</v>
       </c>
       <c r="H63">
-        <v>293964.3</v>
+        <v>258540.1</v>
       </c>
       <c r="I63" t="inlineStr">
         <is>
@@ -4416,7 +4416,7 @@
         <v>15.5</v>
       </c>
       <c r="D64">
-        <v>16.6</v>
+        <v>16.5</v>
       </c>
       <c r="E64">
         <v>17.9</v>
@@ -4425,10 +4425,10 @@
         <v>15.54</v>
       </c>
       <c r="G64">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H64">
-        <v>341094.4</v>
+        <v>340990</v>
       </c>
       <c r="I64" t="inlineStr">
         <is>
@@ -4449,19 +4449,19 @@
         <v>15.5</v>
       </c>
       <c r="D65">
-        <v>16.6</v>
+        <v>16.5</v>
       </c>
       <c r="E65">
-        <v>17.9</v>
+        <v>18.1</v>
       </c>
       <c r="F65">
-        <v>15.51</v>
+        <v>15.5</v>
       </c>
       <c r="G65">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H65">
-        <v>262014.5</v>
+        <v>291440</v>
       </c>
       <c r="I65" t="inlineStr">
         <is>
@@ -4494,7 +4494,7 @@
         <v>-0.14</v>
       </c>
       <c r="H66">
-        <v>284404.7</v>
+        <v>287970.5</v>
       </c>
       <c r="I66" t="inlineStr">
         <is>
@@ -4542,25 +4542,25 @@
         </is>
       </c>
       <c r="B68">
-        <v>40.6</v>
+        <v>40.1</v>
       </c>
       <c r="C68">
         <v>37.7</v>
       </c>
       <c r="D68">
-        <v>40.1</v>
+        <v>39.9</v>
       </c>
       <c r="E68">
-        <v>43.7</v>
+        <v>42.7</v>
       </c>
       <c r="F68">
-        <v>37.67</v>
+        <v>37.65</v>
       </c>
       <c r="G68">
-        <v>-0.43</v>
+        <v>-0.44</v>
       </c>
       <c r="H68">
-        <v>26651.9</v>
+        <v>26140.6</v>
       </c>
       <c r="I68" t="inlineStr">
         <is>
@@ -4578,7 +4578,7 @@
         <v>41.1</v>
       </c>
       <c r="C69">
-        <v>38.5</v>
+        <v>38.4</v>
       </c>
       <c r="D69">
         <v>40.9</v>
@@ -4593,7 +4593,7 @@
         <v>0.35</v>
       </c>
       <c r="H69">
-        <v>28101.3</v>
+        <v>28106.3</v>
       </c>
       <c r="I69" t="inlineStr">
         <is>
@@ -4608,25 +4608,25 @@
         </is>
       </c>
       <c r="B70">
+        <v>40.5</v>
+      </c>
+      <c r="C70">
+        <v>37.5</v>
+      </c>
+      <c r="D70">
         <v>40.1</v>
       </c>
-      <c r="C70">
-        <v>37.6</v>
-      </c>
-      <c r="D70">
-        <v>39.9</v>
-      </c>
       <c r="E70">
-        <v>42.7</v>
+        <v>43.6</v>
       </c>
       <c r="F70">
-        <v>37.56</v>
+        <v>37.54</v>
       </c>
       <c r="G70">
-        <v>-0.53</v>
+        <v>-0.55</v>
       </c>
       <c r="H70">
-        <v>26164.4</v>
+        <v>26650.9</v>
       </c>
       <c r="I70" t="inlineStr">
         <is>
@@ -4653,13 +4653,13 @@
         <v>42.9</v>
       </c>
       <c r="F71">
-        <v>37.69</v>
+        <v>37.73</v>
       </c>
       <c r="G71">
-        <v>-0.4</v>
+        <v>-0.37</v>
       </c>
       <c r="H71">
-        <v>30612</v>
+        <v>30745.5</v>
       </c>
       <c r="I71" t="inlineStr">
         <is>
@@ -4707,25 +4707,25 @@
         </is>
       </c>
       <c r="B73">
-        <v>28.4</v>
+        <v>28</v>
       </c>
       <c r="C73">
         <v>26.1</v>
       </c>
       <c r="D73">
-        <v>28.1</v>
+        <v>27.7</v>
       </c>
       <c r="E73">
-        <v>30.8</v>
+        <v>30</v>
       </c>
       <c r="F73">
-        <v>26.06</v>
+        <v>26.08</v>
       </c>
       <c r="G73">
-        <v>-0.25</v>
+        <v>-0.24</v>
       </c>
       <c r="H73">
-        <v>79985.60000000001</v>
+        <v>77692.89999999999</v>
       </c>
       <c r="I73" t="inlineStr">
         <is>
@@ -4746,19 +4746,19 @@
         <v>26.9</v>
       </c>
       <c r="D74">
-        <v>28.9</v>
+        <v>28.8</v>
       </c>
       <c r="E74">
         <v>31.3</v>
       </c>
       <c r="F74">
-        <v>26.91</v>
+        <v>26.89</v>
       </c>
       <c r="G74">
-        <v>0.59</v>
+        <v>0.57</v>
       </c>
       <c r="H74">
-        <v>87167.10000000001</v>
+        <v>86756.7</v>
       </c>
       <c r="I74" t="inlineStr">
         <is>
@@ -4773,25 +4773,25 @@
         </is>
       </c>
       <c r="B75">
-        <v>27.9</v>
+        <v>28.4</v>
       </c>
       <c r="C75">
         <v>25.8</v>
       </c>
       <c r="D75">
-        <v>27.6</v>
+        <v>28.1</v>
       </c>
       <c r="E75">
-        <v>29.9</v>
+        <v>30.9</v>
       </c>
       <c r="F75">
-        <v>25.76</v>
+        <v>25.82</v>
       </c>
       <c r="G75">
-        <v>-0.55</v>
+        <v>-0.5</v>
       </c>
       <c r="H75">
-        <v>76880</v>
+        <v>80342</v>
       </c>
       <c r="I75" t="inlineStr">
         <is>
@@ -4818,13 +4818,13 @@
         <v>31</v>
       </c>
       <c r="F76">
-        <v>26.73</v>
+        <v>26.74</v>
       </c>
       <c r="G76">
-        <v>0.41</v>
+        <v>0.43</v>
       </c>
       <c r="H76">
-        <v>141011.4</v>
+        <v>140491.6</v>
       </c>
       <c r="I76" t="inlineStr">
         <is>
@@ -4872,16 +4872,16 @@
         </is>
       </c>
       <c r="B78">
-        <v>23.2</v>
+        <v>23</v>
       </c>
       <c r="C78">
         <v>21.6</v>
       </c>
       <c r="D78">
-        <v>22.7</v>
+        <v>22.6</v>
       </c>
       <c r="E78">
-        <v>25</v>
+        <v>24.6</v>
       </c>
       <c r="F78">
         <v>21.62</v>
@@ -4890,7 +4890,7 @@
         <v>-0.24</v>
       </c>
       <c r="H78">
-        <v>59397</v>
+        <v>57215.1</v>
       </c>
       <c r="I78" t="inlineStr">
         <is>
@@ -4911,19 +4911,19 @@
         <v>22.3</v>
       </c>
       <c r="D79">
-        <v>23.4</v>
+        <v>23.3</v>
       </c>
       <c r="E79">
         <v>25.3</v>
       </c>
       <c r="F79">
-        <v>22.26</v>
+        <v>22.25</v>
       </c>
       <c r="G79">
-        <v>0.4</v>
+        <v>0.39</v>
       </c>
       <c r="H79">
-        <v>63834.8</v>
+        <v>64052.2</v>
       </c>
       <c r="I79" t="inlineStr">
         <is>
@@ -4938,16 +4938,16 @@
         </is>
       </c>
       <c r="B80">
-        <v>23</v>
+        <v>23.1</v>
       </c>
       <c r="C80">
         <v>21.6</v>
       </c>
       <c r="D80">
-        <v>22.6</v>
+        <v>22.7</v>
       </c>
       <c r="E80">
-        <v>24.6</v>
+        <v>25</v>
       </c>
       <c r="F80">
         <v>21.56</v>
@@ -4956,7 +4956,7 @@
         <v>-0.3</v>
       </c>
       <c r="H80">
-        <v>57355.5</v>
+        <v>59442.1</v>
       </c>
       <c r="I80" t="inlineStr">
         <is>
@@ -4971,10 +4971,10 @@
         </is>
       </c>
       <c r="B81">
-        <v>22.8</v>
+        <v>22.9</v>
       </c>
       <c r="C81">
-        <v>21.5</v>
+        <v>21.6</v>
       </c>
       <c r="D81">
         <v>22.6</v>
@@ -4983,13 +4983,13 @@
         <v>24.4</v>
       </c>
       <c r="F81">
-        <v>21.53</v>
+        <v>21.6</v>
       </c>
       <c r="G81">
-        <v>-0.33</v>
+        <v>-0.26</v>
       </c>
       <c r="H81">
-        <v>69908</v>
+        <v>69724.8</v>
       </c>
       <c r="I81" t="inlineStr">
         <is>
@@ -5037,25 +5037,25 @@
         </is>
       </c>
       <c r="B83">
-        <v>33.2</v>
+        <v>32.6</v>
       </c>
       <c r="C83">
-        <v>31.7</v>
+        <v>31.4</v>
       </c>
       <c r="D83">
-        <v>32.9</v>
+        <v>32.3</v>
       </c>
       <c r="E83">
-        <v>34.8</v>
+        <v>34</v>
       </c>
       <c r="F83">
-        <v>31.74</v>
+        <v>31.75</v>
       </c>
       <c r="G83">
-        <v>-0.26</v>
+        <v>-0.25</v>
       </c>
       <c r="H83">
-        <v>417495.2</v>
+        <v>396584.2</v>
       </c>
       <c r="I83" t="inlineStr">
         <is>
@@ -5082,13 +5082,13 @@
         <v>36</v>
       </c>
       <c r="F84">
-        <v>32.95</v>
+        <v>32.96</v>
       </c>
       <c r="G84">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="H84">
-        <v>456489.4</v>
+        <v>456895.7</v>
       </c>
       <c r="I84" t="inlineStr">
         <is>
@@ -5103,25 +5103,25 @@
         </is>
       </c>
       <c r="B85">
-        <v>32.5</v>
+        <v>33.1</v>
       </c>
       <c r="C85">
         <v>31.2</v>
       </c>
       <c r="D85">
-        <v>32.3</v>
+        <v>32.9</v>
       </c>
       <c r="E85">
-        <v>34</v>
+        <v>34.8</v>
       </c>
       <c r="F85">
-        <v>31.2</v>
+        <v>31.21</v>
       </c>
       <c r="G85">
-        <v>-0.8</v>
+        <v>-0.79</v>
       </c>
       <c r="H85">
-        <v>396086.4</v>
+        <v>417721.6</v>
       </c>
       <c r="I85" t="inlineStr">
         <is>
@@ -5136,7 +5136,7 @@
         </is>
       </c>
       <c r="B86">
-        <v>33</v>
+        <v>33.1</v>
       </c>
       <c r="C86">
         <v>31.7</v>
@@ -5148,13 +5148,13 @@
         <v>34.6</v>
       </c>
       <c r="F86">
-        <v>31.73</v>
+        <v>31.74</v>
       </c>
       <c r="G86">
-        <v>-0.27</v>
+        <v>-0.26</v>
       </c>
       <c r="H86">
-        <v>449972</v>
+        <v>450824.8</v>
       </c>
       <c r="I86" t="inlineStr">
         <is>
@@ -5202,25 +5202,25 @@
         </is>
       </c>
       <c r="B88">
-        <v>29.7</v>
+        <v>28.8</v>
       </c>
       <c r="C88">
-        <v>27.7</v>
+        <v>27.3</v>
       </c>
       <c r="D88">
-        <v>29.3</v>
+        <v>28.2</v>
       </c>
       <c r="E88">
-        <v>32.3</v>
+        <v>30.9</v>
       </c>
       <c r="F88">
-        <v>27.69</v>
+        <v>27.68</v>
       </c>
       <c r="G88">
-        <v>-0.31</v>
+        <v>-0.32</v>
       </c>
       <c r="H88">
-        <v>2722312.2</v>
+        <v>2593675.4</v>
       </c>
       <c r="I88" t="inlineStr">
         <is>
@@ -5241,19 +5241,19 @@
         <v>29.3</v>
       </c>
       <c r="D89">
-        <v>30.9</v>
+        <v>30.8</v>
       </c>
       <c r="E89">
-        <v>33.9</v>
+        <v>33.8</v>
       </c>
       <c r="F89">
-        <v>29.32</v>
+        <v>29.29</v>
       </c>
       <c r="G89">
-        <v>1.32</v>
+        <v>1.29</v>
       </c>
       <c r="H89">
-        <v>2957194.8</v>
+        <v>2969372.6</v>
       </c>
       <c r="I89" t="inlineStr">
         <is>
@@ -5268,25 +5268,25 @@
         </is>
       </c>
       <c r="B90">
-        <v>28.5</v>
+        <v>29.5</v>
       </c>
       <c r="C90">
         <v>26.8</v>
       </c>
       <c r="D90">
-        <v>28.2</v>
+        <v>29.3</v>
       </c>
       <c r="E90">
-        <v>30.9</v>
+        <v>32.3</v>
       </c>
       <c r="F90">
-        <v>26.76</v>
+        <v>26.8</v>
       </c>
       <c r="G90">
-        <v>-1.24</v>
+        <v>-1.2</v>
       </c>
       <c r="H90">
-        <v>2542699.8</v>
+        <v>2726886.6</v>
       </c>
       <c r="I90" t="inlineStr">
         <is>
@@ -5313,13 +5313,13 @@
         <v>32.3</v>
       </c>
       <c r="F91">
-        <v>28.13</v>
+        <v>28.12</v>
       </c>
       <c r="G91">
-        <v>0.13</v>
+        <v>0.12</v>
       </c>
       <c r="H91">
-        <v>3500739.2</v>
+        <v>3504749.4</v>
       </c>
       <c r="I91" t="inlineStr">
         <is>
@@ -5367,16 +5367,16 @@
         </is>
       </c>
       <c r="B93">
-        <v>34.1</v>
+        <v>33.8</v>
       </c>
       <c r="C93">
         <v>31.6</v>
       </c>
       <c r="D93">
-        <v>33.7</v>
+        <v>33.4</v>
       </c>
       <c r="E93">
-        <v>36.9</v>
+        <v>36</v>
       </c>
       <c r="F93">
         <v>31.56</v>
@@ -5385,7 +5385,7 @@
         <v>-0.34</v>
       </c>
       <c r="H93">
-        <v>8888</v>
+        <v>8725</v>
       </c>
       <c r="I93" t="inlineStr">
         <is>
@@ -5412,13 +5412,13 @@
         <v>36.8</v>
       </c>
       <c r="F94">
-        <v>32.07</v>
+        <v>32.06</v>
       </c>
       <c r="G94">
-        <v>0.18</v>
+        <v>0.17</v>
       </c>
       <c r="H94">
-        <v>9232.1</v>
+        <v>9227.700000000001</v>
       </c>
       <c r="I94" t="inlineStr">
         <is>
@@ -5433,25 +5433,25 @@
         </is>
       </c>
       <c r="B95">
-        <v>33.7</v>
+        <v>34.1</v>
       </c>
       <c r="C95">
-        <v>31.4</v>
+        <v>31.5</v>
       </c>
       <c r="D95">
-        <v>33.4</v>
+        <v>33.6</v>
       </c>
       <c r="E95">
-        <v>35.9</v>
+        <v>36.9</v>
       </c>
       <c r="F95">
-        <v>31.42</v>
+        <v>31.48</v>
       </c>
       <c r="G95">
-        <v>-0.48</v>
+        <v>-0.42</v>
       </c>
       <c r="H95">
-        <v>8677.299999999999</v>
+        <v>8891.299999999999</v>
       </c>
       <c r="I95" t="inlineStr">
         <is>
@@ -5478,13 +5478,13 @@
         <v>36.2</v>
       </c>
       <c r="F96">
-        <v>31.57</v>
+        <v>31.59</v>
       </c>
       <c r="G96">
-        <v>-0.33</v>
+        <v>-0.31</v>
       </c>
       <c r="H96">
-        <v>9850.299999999999</v>
+        <v>9930.299999999999</v>
       </c>
       <c r="I96" t="inlineStr">
         <is>
@@ -5532,7 +5532,7 @@
         </is>
       </c>
       <c r="B98">
-        <v>36.6</v>
+        <v>36.4</v>
       </c>
       <c r="C98">
         <v>34</v>
@@ -5541,16 +5541,16 @@
         <v>36.1</v>
       </c>
       <c r="E98">
-        <v>39.4</v>
+        <v>38.7</v>
       </c>
       <c r="F98">
-        <v>34.03</v>
+        <v>34.04</v>
       </c>
       <c r="G98">
-        <v>-0.42</v>
+        <v>-0.4</v>
       </c>
       <c r="H98">
-        <v>8574.1</v>
+        <v>8505.5</v>
       </c>
       <c r="I98" t="inlineStr">
         <is>
@@ -5577,13 +5577,13 @@
         <v>39.1</v>
       </c>
       <c r="F99">
-        <v>34.53</v>
+        <v>34.52</v>
       </c>
       <c r="G99">
-        <v>0.08</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="H99">
-        <v>8865.6</v>
+        <v>8894.200000000001</v>
       </c>
       <c r="I99" t="inlineStr">
         <is>
@@ -5598,7 +5598,7 @@
         </is>
       </c>
       <c r="B100">
-        <v>36.4</v>
+        <v>36.6</v>
       </c>
       <c r="C100">
         <v>34.2</v>
@@ -5607,7 +5607,7 @@
         <v>36.1</v>
       </c>
       <c r="E100">
-        <v>38.6</v>
+        <v>39.4</v>
       </c>
       <c r="F100">
         <v>34.2</v>
@@ -5616,7 +5616,7 @@
         <v>-0.25</v>
       </c>
       <c r="H100">
-        <v>8431</v>
+        <v>8585.799999999999</v>
       </c>
       <c r="I100" t="inlineStr">
         <is>
@@ -5643,13 +5643,13 @@
         <v>38.5</v>
       </c>
       <c r="F101">
-        <v>34.06</v>
+        <v>34.07</v>
       </c>
       <c r="G101">
-        <v>-0.39</v>
+        <v>-0.38</v>
       </c>
       <c r="H101">
-        <v>9456.5</v>
+        <v>9491.6</v>
       </c>
       <c r="I101" t="inlineStr">
         <is>
@@ -5697,25 +5697,25 @@
         </is>
       </c>
       <c r="B103">
-        <v>60.5</v>
+        <v>58.3</v>
       </c>
       <c r="C103">
-        <v>54.6</v>
+        <v>54.1</v>
       </c>
       <c r="D103">
-        <v>59.3</v>
+        <v>57.1</v>
       </c>
       <c r="E103">
-        <v>66.2</v>
+        <v>63.1</v>
       </c>
       <c r="F103">
-        <v>54.63</v>
+        <v>54.64</v>
       </c>
       <c r="G103">
-        <v>-0.37</v>
+        <v>-0.36</v>
       </c>
       <c r="H103">
-        <v>388200.1</v>
+        <v>338016.6</v>
       </c>
       <c r="I103" t="inlineStr">
         <is>
@@ -5730,25 +5730,25 @@
         </is>
       </c>
       <c r="B104">
-        <v>63.5</v>
+        <v>63.4</v>
       </c>
       <c r="C104">
-        <v>57.8</v>
+        <v>57.7</v>
       </c>
       <c r="D104">
-        <v>62.3</v>
+        <v>62.2</v>
       </c>
       <c r="E104">
-        <v>68.8</v>
+        <v>68.7</v>
       </c>
       <c r="F104">
-        <v>57.85</v>
+        <v>57.73</v>
       </c>
       <c r="G104">
-        <v>2.85</v>
+        <v>2.73</v>
       </c>
       <c r="H104">
-        <v>487932.1</v>
+        <v>484473.9</v>
       </c>
       <c r="I104" t="inlineStr">
         <is>
@@ -5763,25 +5763,25 @@
         </is>
       </c>
       <c r="B105">
-        <v>58.2</v>
+        <v>60.3</v>
       </c>
       <c r="C105">
-        <v>53.2</v>
+        <v>53</v>
       </c>
       <c r="D105">
-        <v>57.3</v>
+        <v>59.3</v>
       </c>
       <c r="E105">
-        <v>63.2</v>
+        <v>66.3</v>
       </c>
       <c r="F105">
-        <v>53.21</v>
+        <v>53.04</v>
       </c>
       <c r="G105">
-        <v>-1.79</v>
+        <v>-1.96</v>
       </c>
       <c r="H105">
-        <v>343146.4</v>
+        <v>388626.7</v>
       </c>
       <c r="I105" t="inlineStr">
         <is>
@@ -5796,25 +5796,25 @@
         </is>
       </c>
       <c r="B106">
-        <v>59.7</v>
+        <v>59.6</v>
       </c>
       <c r="C106">
         <v>54.4</v>
       </c>
       <c r="D106">
-        <v>58.6</v>
+        <v>58.5</v>
       </c>
       <c r="E106">
         <v>64.7</v>
       </c>
       <c r="F106">
-        <v>54.43</v>
+        <v>54.37</v>
       </c>
       <c r="G106">
-        <v>-0.57</v>
+        <v>-0.63</v>
       </c>
       <c r="H106">
-        <v>384853.7</v>
+        <v>382943</v>
       </c>
       <c r="I106" t="inlineStr">
         <is>
@@ -5862,7 +5862,7 @@
         </is>
       </c>
       <c r="B108">
-        <v>33.1</v>
+        <v>32.9</v>
       </c>
       <c r="C108">
         <v>32</v>
@@ -5871,16 +5871,16 @@
         <v>32</v>
       </c>
       <c r="E108">
-        <v>35.2</v>
+        <v>34.5</v>
       </c>
       <c r="F108">
-        <v>32.04</v>
+        <v>32.01</v>
       </c>
       <c r="G108">
-        <v>-0.34</v>
+        <v>-0.37</v>
       </c>
       <c r="H108">
-        <v>2117441.3</v>
+        <v>2116302.5</v>
       </c>
       <c r="I108" t="inlineStr">
         <is>
@@ -5895,25 +5895,25 @@
         </is>
       </c>
       <c r="B109">
-        <v>37.1</v>
+        <v>36.6</v>
       </c>
       <c r="C109">
-        <v>36.1</v>
+        <v>35.6</v>
       </c>
       <c r="D109">
-        <v>36.1</v>
+        <v>35.6</v>
       </c>
       <c r="E109">
-        <v>38.9</v>
+        <v>38.4</v>
       </c>
       <c r="F109">
-        <v>36.09</v>
+        <v>35.63</v>
       </c>
       <c r="G109">
-        <v>3.71</v>
+        <v>3.25</v>
       </c>
       <c r="H109">
-        <v>2694343.8</v>
+        <v>2632264.5</v>
       </c>
       <c r="I109" t="inlineStr">
         <is>
@@ -5928,25 +5928,25 @@
         </is>
       </c>
       <c r="B110">
-        <v>33</v>
+        <v>33.1</v>
       </c>
       <c r="C110">
-        <v>32.1</v>
+        <v>32</v>
       </c>
       <c r="D110">
-        <v>32.1</v>
+        <v>32</v>
       </c>
       <c r="E110">
-        <v>34.5</v>
+        <v>35.1</v>
       </c>
       <c r="F110">
-        <v>32.09</v>
+        <v>32.03</v>
       </c>
       <c r="G110">
-        <v>-0.29</v>
+        <v>-0.35</v>
       </c>
       <c r="H110">
-        <v>2119750.7</v>
+        <v>2114583.8</v>
       </c>
       <c r="I110" t="inlineStr">
         <is>
@@ -5964,22 +5964,22 @@
         <v>32.4</v>
       </c>
       <c r="C111">
-        <v>31.5</v>
+        <v>31.6</v>
       </c>
       <c r="D111">
-        <v>31.5</v>
+        <v>31.6</v>
       </c>
       <c r="E111">
         <v>34</v>
       </c>
       <c r="F111">
-        <v>31.55</v>
+        <v>31.56</v>
       </c>
       <c r="G111">
-        <v>-0.83</v>
+        <v>-0.82</v>
       </c>
       <c r="H111">
-        <v>2084559.9</v>
+        <v>2085942.9</v>
       </c>
       <c r="I111" t="inlineStr">
         <is>
@@ -6027,7 +6027,7 @@
         </is>
       </c>
       <c r="B113">
-        <v>15.9</v>
+        <v>15.8</v>
       </c>
       <c r="C113">
         <v>14.7</v>
@@ -6036,7 +6036,7 @@
         <v>15.4</v>
       </c>
       <c r="E113">
-        <v>17.1</v>
+        <v>17</v>
       </c>
       <c r="F113">
         <v>14.71</v>
@@ -6045,7 +6045,7 @@
         <v>-0.15</v>
       </c>
       <c r="H113">
-        <v>1748485.7</v>
+        <v>1736315</v>
       </c>
       <c r="I113" t="inlineStr">
         <is>
@@ -6078,7 +6078,7 @@
         <v>-0.09</v>
       </c>
       <c r="H114">
-        <v>1818676.7</v>
+        <v>1810657.2</v>
       </c>
       <c r="I114" t="inlineStr">
         <is>
@@ -6102,16 +6102,16 @@
         <v>15.4</v>
       </c>
       <c r="E115">
-        <v>17</v>
+        <v>17.1</v>
       </c>
       <c r="F115">
-        <v>14.83</v>
+        <v>14.82</v>
       </c>
       <c r="G115">
-        <v>-0.03</v>
+        <v>-0.04</v>
       </c>
       <c r="H115">
-        <v>1736083.1</v>
+        <v>1742573.5</v>
       </c>
       <c r="I115" t="inlineStr">
         <is>
@@ -6132,19 +6132,19 @@
         <v>14.9</v>
       </c>
       <c r="D116">
-        <v>15.5</v>
+        <v>15.4</v>
       </c>
       <c r="E116">
         <v>17.1</v>
       </c>
       <c r="F116">
-        <v>14.88</v>
+        <v>14.86</v>
       </c>
       <c r="G116">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="H116">
-        <v>1764447.9</v>
+        <v>1759289.8</v>
       </c>
       <c r="I116" t="inlineStr">
         <is>
@@ -6192,25 +6192,25 @@
         </is>
       </c>
       <c r="B118">
-        <v>108.5</v>
+        <v>107.7</v>
       </c>
       <c r="C118">
-        <v>103.4</v>
+        <v>103.2</v>
       </c>
       <c r="D118">
-        <v>105.7</v>
+        <v>105.3</v>
       </c>
       <c r="E118">
-        <v>117.6</v>
+        <v>115.6</v>
       </c>
       <c r="F118">
-        <v>103.41</v>
+        <v>103.24</v>
       </c>
       <c r="G118">
-        <v>-1.59</v>
+        <v>-1.76</v>
       </c>
       <c r="H118">
-        <v>3885930.4</v>
+        <v>3899250</v>
       </c>
       <c r="I118" t="inlineStr">
         <is>
@@ -6225,25 +6225,25 @@
         </is>
       </c>
       <c r="B119">
-        <v>111.8</v>
+        <v>111.9</v>
       </c>
       <c r="C119">
-        <v>107</v>
+        <v>107.1</v>
       </c>
       <c r="D119">
-        <v>109.4</v>
+        <v>109.5</v>
       </c>
       <c r="E119">
-        <v>120.4</v>
+        <v>120.7</v>
       </c>
       <c r="F119">
-        <v>107.04</v>
+        <v>107.08</v>
       </c>
       <c r="G119">
-        <v>2.04</v>
+        <v>2.08</v>
       </c>
       <c r="H119">
-        <v>4040523.4</v>
+        <v>4042695.7</v>
       </c>
       <c r="I119" t="inlineStr">
         <is>
@@ -6258,25 +6258,25 @@
         </is>
       </c>
       <c r="B120">
-        <v>108.5</v>
+        <v>108.2</v>
       </c>
       <c r="C120">
-        <v>103.9</v>
+        <v>103</v>
       </c>
       <c r="D120">
-        <v>106.2</v>
+        <v>105.6</v>
       </c>
       <c r="E120">
-        <v>116.8</v>
+        <v>117.6</v>
       </c>
       <c r="F120">
-        <v>103.87</v>
+        <v>102.96</v>
       </c>
       <c r="G120">
-        <v>-1.13</v>
+        <v>-2.04</v>
       </c>
       <c r="H120">
-        <v>3909321.5</v>
+        <v>3884479.9</v>
       </c>
       <c r="I120" t="inlineStr">
         <is>
@@ -6291,25 +6291,25 @@
         </is>
       </c>
       <c r="B121">
-        <v>107.8</v>
+        <v>108.1</v>
       </c>
       <c r="C121">
-        <v>103.2</v>
+        <v>103.6</v>
       </c>
       <c r="D121">
-        <v>105.6</v>
+        <v>105.9</v>
       </c>
       <c r="E121">
-        <v>115.9</v>
+        <v>116.3</v>
       </c>
       <c r="F121">
-        <v>103.25</v>
+        <v>103.58</v>
       </c>
       <c r="G121">
-        <v>-1.75</v>
+        <v>-1.42</v>
       </c>
       <c r="H121">
-        <v>4119062.6</v>
+        <v>4126374.9</v>
       </c>
       <c r="I121" t="inlineStr">
         <is>
@@ -6357,16 +6357,16 @@
         </is>
       </c>
       <c r="B123">
-        <v>34.1</v>
+        <v>33.7</v>
       </c>
       <c r="C123">
         <v>32.5</v>
       </c>
       <c r="D123">
-        <v>33.4</v>
+        <v>33</v>
       </c>
       <c r="E123">
-        <v>36.5</v>
+        <v>35.6</v>
       </c>
       <c r="F123">
         <v>32.53</v>
@@ -6375,7 +6375,7 @@
         <v>-0.22</v>
       </c>
       <c r="H123">
-        <v>217618.6</v>
+        <v>208515.3</v>
       </c>
       <c r="I123" t="inlineStr">
         <is>
@@ -6390,25 +6390,25 @@
         </is>
       </c>
       <c r="B124">
-        <v>39.7</v>
+        <v>39.4</v>
       </c>
       <c r="C124">
-        <v>38</v>
+        <v>37.7</v>
       </c>
       <c r="D124">
-        <v>39</v>
+        <v>38.7</v>
       </c>
       <c r="E124">
-        <v>42</v>
+        <v>41.7</v>
       </c>
       <c r="F124">
-        <v>37.98</v>
+        <v>37.7</v>
       </c>
       <c r="G124">
-        <v>5.23</v>
+        <v>4.95</v>
       </c>
       <c r="H124">
-        <v>335537.3</v>
+        <v>329844.7</v>
       </c>
       <c r="I124" t="inlineStr">
         <is>
@@ -6423,25 +6423,25 @@
         </is>
       </c>
       <c r="B125">
-        <v>33.6</v>
+        <v>34.1</v>
       </c>
       <c r="C125">
         <v>32.2</v>
       </c>
       <c r="D125">
-        <v>33.1</v>
+        <v>33.4</v>
       </c>
       <c r="E125">
-        <v>35.7</v>
+        <v>36.5</v>
       </c>
       <c r="F125">
-        <v>32.23</v>
+        <v>32.21</v>
       </c>
       <c r="G125">
-        <v>-0.52</v>
+        <v>-0.54</v>
       </c>
       <c r="H125">
-        <v>206331.1</v>
+        <v>217606.3</v>
       </c>
       <c r="I125" t="inlineStr">
         <is>
@@ -6456,25 +6456,25 @@
         </is>
       </c>
       <c r="B126">
-        <v>34</v>
+        <v>33.9</v>
       </c>
       <c r="C126">
-        <v>32.6</v>
+        <v>32.5</v>
       </c>
       <c r="D126">
-        <v>33.5</v>
+        <v>33.4</v>
       </c>
       <c r="E126">
-        <v>36</v>
+        <v>35.9</v>
       </c>
       <c r="F126">
-        <v>32.65</v>
+        <v>32.53</v>
       </c>
       <c r="G126">
-        <v>-0.1</v>
+        <v>-0.22</v>
       </c>
       <c r="H126">
-        <v>232812</v>
+        <v>228891.4</v>
       </c>
       <c r="I126" t="inlineStr">
         <is>
@@ -6522,25 +6522,25 @@
         </is>
       </c>
       <c r="B128">
-        <v>11.2</v>
+        <v>11</v>
       </c>
       <c r="C128">
         <v>10.7</v>
       </c>
       <c r="D128">
-        <v>11.1</v>
+        <v>10.8</v>
       </c>
       <c r="E128">
-        <v>12</v>
+        <v>11.6</v>
       </c>
       <c r="F128">
-        <v>10.73</v>
+        <v>10.72</v>
       </c>
       <c r="G128">
-        <v>-0.06</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="H128">
-        <v>6834.4</v>
+        <v>6297.4</v>
       </c>
       <c r="I128" t="inlineStr">
         <is>
@@ -6555,25 +6555,25 @@
         </is>
       </c>
       <c r="B129">
-        <v>12.1</v>
+        <v>12</v>
       </c>
       <c r="C129">
-        <v>11.6</v>
+        <v>11.5</v>
       </c>
       <c r="D129">
-        <v>12</v>
+        <v>11.9</v>
       </c>
       <c r="E129">
-        <v>12.8</v>
+        <v>12.7</v>
       </c>
       <c r="F129">
-        <v>11.64</v>
+        <v>11.55</v>
       </c>
       <c r="G129">
-        <v>0.85</v>
+        <v>0.76</v>
       </c>
       <c r="H129">
-        <v>9399.700000000001</v>
+        <v>9152.799999999999</v>
       </c>
       <c r="I129" t="inlineStr">
         <is>
@@ -6588,25 +6588,25 @@
         </is>
       </c>
       <c r="B130">
-        <v>11</v>
+        <v>11.2</v>
       </c>
       <c r="C130">
-        <v>10.6</v>
+        <v>10.5</v>
       </c>
       <c r="D130">
-        <v>10.9</v>
+        <v>11.1</v>
       </c>
       <c r="E130">
-        <v>11.6</v>
+        <v>12</v>
       </c>
       <c r="F130">
-        <v>10.59</v>
+        <v>10.54</v>
       </c>
       <c r="G130">
-        <v>-0.2</v>
+        <v>-0.25</v>
       </c>
       <c r="H130">
-        <v>6445.5</v>
+        <v>6825.6</v>
       </c>
       <c r="I130" t="inlineStr">
         <is>
@@ -6621,25 +6621,25 @@
         </is>
       </c>
       <c r="B131">
+        <v>11</v>
+      </c>
+      <c r="C131">
+        <v>10.6</v>
+      </c>
+      <c r="D131">
         <v>10.9</v>
       </c>
-      <c r="C131">
-        <v>10.5</v>
-      </c>
-      <c r="D131">
-        <v>10.8</v>
-      </c>
       <c r="E131">
-        <v>11.5</v>
+        <v>11.6</v>
       </c>
       <c r="F131">
-        <v>10.52</v>
+        <v>10.6</v>
       </c>
       <c r="G131">
-        <v>-0.27</v>
+        <v>-0.19</v>
       </c>
       <c r="H131">
-        <v>6259</v>
+        <v>6493.2</v>
       </c>
       <c r="I131" t="inlineStr">
         <is>
@@ -6687,16 +6687,16 @@
         </is>
       </c>
       <c r="B133">
-        <v>6.6</v>
+        <v>6.4</v>
       </c>
       <c r="C133">
         <v>5.9</v>
       </c>
       <c r="D133">
-        <v>6.5</v>
+        <v>6.3</v>
       </c>
       <c r="E133">
-        <v>7.2</v>
+        <v>7</v>
       </c>
       <c r="F133">
         <v>5.89</v>
@@ -6705,7 +6705,7 @@
         <v>-0.02</v>
       </c>
       <c r="H133">
-        <v>494683.9</v>
+        <v>443933.3</v>
       </c>
       <c r="I133" t="inlineStr">
         <is>
@@ -6732,13 +6732,13 @@
         <v>7.4</v>
       </c>
       <c r="F134">
-        <v>6.1</v>
+        <v>6.08</v>
       </c>
       <c r="G134">
-        <v>0.19</v>
+        <v>0.17</v>
       </c>
       <c r="H134">
-        <v>570903.9</v>
+        <v>564421.1</v>
       </c>
       <c r="I134" t="inlineStr">
         <is>
@@ -6753,16 +6753,16 @@
         </is>
       </c>
       <c r="B135">
-        <v>6.4</v>
+        <v>6.6</v>
       </c>
       <c r="C135">
-        <v>5.8</v>
+        <v>5.9</v>
       </c>
       <c r="D135">
-        <v>6.3</v>
+        <v>6.5</v>
       </c>
       <c r="E135">
-        <v>7</v>
+        <v>7.2</v>
       </c>
       <c r="F135">
         <v>5.76</v>
@@ -6771,7 +6771,7 @@
         <v>-0.15</v>
       </c>
       <c r="H135">
-        <v>445449</v>
+        <v>493921.8</v>
       </c>
       <c r="I135" t="inlineStr">
         <is>
@@ -6804,7 +6804,7 @@
         <v>-0.06</v>
       </c>
       <c r="H136">
-        <v>480470.6</v>
+        <v>481812.4</v>
       </c>
       <c r="I136" t="inlineStr">
         <is>
@@ -6852,25 +6852,25 @@
         </is>
       </c>
       <c r="B138">
-        <v>14.7</v>
+        <v>14.3</v>
       </c>
       <c r="C138">
-        <v>13.9</v>
+        <v>13.7</v>
       </c>
       <c r="D138">
-        <v>14.5</v>
+        <v>14.1</v>
       </c>
       <c r="E138">
-        <v>15.7</v>
+        <v>15</v>
       </c>
       <c r="F138">
-        <v>13.92</v>
+        <v>13.88</v>
       </c>
       <c r="G138">
-        <v>-0.08</v>
+        <v>-0.12</v>
       </c>
       <c r="H138">
-        <v>403289.8</v>
+        <v>363315.7</v>
       </c>
       <c r="I138" t="inlineStr">
         <is>
@@ -6897,13 +6897,13 @@
         <v>16.3</v>
       </c>
       <c r="F139">
-        <v>14.7</v>
+        <v>14.68</v>
       </c>
       <c r="G139">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
       <c r="H139">
-        <v>500335.8</v>
+        <v>497761.3</v>
       </c>
       <c r="I139" t="inlineStr">
         <is>
@@ -6918,25 +6918,25 @@
         </is>
       </c>
       <c r="B140">
+        <v>14.6</v>
+      </c>
+      <c r="C140">
+        <v>13.6</v>
+      </c>
+      <c r="D140">
         <v>14.4</v>
       </c>
-      <c r="C140">
-        <v>13.7</v>
-      </c>
-      <c r="D140">
-        <v>14.2</v>
-      </c>
       <c r="E140">
-        <v>15.1</v>
+        <v>15.8</v>
       </c>
       <c r="F140">
-        <v>13.71</v>
+        <v>13.62</v>
       </c>
       <c r="G140">
-        <v>-0.29</v>
+        <v>-0.38</v>
       </c>
       <c r="H140">
-        <v>375481</v>
+        <v>398600.3</v>
       </c>
       <c r="I140" t="inlineStr">
         <is>
@@ -6951,25 +6951,25 @@
         </is>
       </c>
       <c r="B141">
-        <v>14.4</v>
+        <v>14.3</v>
       </c>
       <c r="C141">
-        <v>13.8</v>
+        <v>13.7</v>
       </c>
       <c r="D141">
-        <v>14.2</v>
+        <v>14.1</v>
       </c>
       <c r="E141">
-        <v>15.2</v>
+        <v>15.1</v>
       </c>
       <c r="F141">
-        <v>13.75</v>
+        <v>13.65</v>
       </c>
       <c r="G141">
-        <v>-0.25</v>
+        <v>-0.35</v>
       </c>
       <c r="H141">
-        <v>383645.5</v>
+        <v>371165.8</v>
       </c>
       <c r="I141" t="inlineStr">
         <is>

</xml_diff>